<commit_message>
Update FORMATO 7C IES JOSÉ MARIA ARGUEDAS CHUQUIBAMBILLA.xlsx
</commit_message>
<xml_diff>
--- a/13.0 FORMATO N°07 INVIERTE PE/FORMATO 7C IES JOSÉ MARIA ARGUEDAS CHUQUIBAMBILLA.xlsx
+++ b/13.0 FORMATO N°07 INVIERTE PE/FORMATO 7C IES JOSÉ MARIA ARGUEDAS CHUQUIBAMBILLA.xlsx
@@ -2014,6 +2014,327 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2026,21 +2347,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2050,87 +2362,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2139,246 +2379,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2666,7 +2666,7 @@
   <dimension ref="B3:Q547"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A470" zoomScale="70" zoomScaleNormal="51" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="N488" sqref="N488"/>
+      <selection activeCell="I488" sqref="I488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2688,52 +2688,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="214" t="s">
+      <c r="B3" s="191" t="s">
         <v>258</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="216"/>
-      <c r="I3" s="216"/>
-      <c r="J3" s="216"/>
-      <c r="K3" s="216"/>
-      <c r="L3" s="216"/>
-      <c r="M3" s="217"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="193"/>
+      <c r="H3" s="193"/>
+      <c r="I3" s="193"/>
+      <c r="J3" s="193"/>
+      <c r="K3" s="193"/>
+      <c r="L3" s="193"/>
+      <c r="M3" s="194"/>
     </row>
     <row r="4" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="218" t="s">
+      <c r="B4" s="195" t="s">
         <v>259</v>
       </c>
-      <c r="C4" s="219"/>
-      <c r="D4" s="220"/>
-      <c r="E4" s="220"/>
-      <c r="F4" s="220"/>
-      <c r="G4" s="220"/>
-      <c r="H4" s="220"/>
-      <c r="I4" s="220"/>
-      <c r="J4" s="220"/>
-      <c r="K4" s="220"/>
-      <c r="L4" s="220"/>
-      <c r="M4" s="221"/>
+      <c r="C4" s="196"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="198"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="222" t="s">
+      <c r="B5" s="172" t="s">
         <v>261</v>
       </c>
-      <c r="C5" s="222"/>
-      <c r="D5" s="223"/>
-      <c r="E5" s="223"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="223"/>
-      <c r="H5" s="223"/>
-      <c r="I5" s="223"/>
-      <c r="J5" s="223"/>
-      <c r="K5" s="223"/>
-      <c r="L5" s="223"/>
-      <c r="M5" s="223"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="199"/>
+      <c r="M5" s="199"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -2767,17 +2767,17 @@
     </row>
     <row r="8" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="256" t="s">
+      <c r="C8" s="242" t="s">
         <v>336</v>
       </c>
-      <c r="D8" s="257"/>
-      <c r="E8" s="257"/>
-      <c r="F8" s="257"/>
-      <c r="G8" s="257"/>
-      <c r="H8" s="257"/>
-      <c r="I8" s="257"/>
-      <c r="J8" s="257"/>
-      <c r="K8" s="258"/>
+      <c r="D8" s="243"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="243"/>
+      <c r="I8" s="243"/>
+      <c r="J8" s="243"/>
+      <c r="K8" s="244"/>
       <c r="L8" s="155"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -3071,13 +3071,13 @@
       </c>
       <c r="D27" s="92"/>
       <c r="E27" s="92"/>
-      <c r="G27" s="259" t="s">
+      <c r="G27" s="245" t="s">
         <v>330</v>
       </c>
-      <c r="H27" s="259"/>
-      <c r="I27" s="259"/>
-      <c r="J27" s="259"/>
-      <c r="K27" s="259"/>
+      <c r="H27" s="245"/>
+      <c r="I27" s="245"/>
+      <c r="J27" s="245"/>
+      <c r="K27" s="245"/>
       <c r="L27" s="156"/>
       <c r="M27" s="80"/>
     </row>
@@ -3096,22 +3096,22 @@
     </row>
     <row r="29" spans="2:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="89"/>
-      <c r="C29" s="224" t="s">
+      <c r="C29" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="224"/>
-      <c r="E29" s="224"/>
+      <c r="D29" s="200"/>
+      <c r="E29" s="200"/>
       <c r="G29" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="260" t="s">
+      <c r="H29" s="246" t="s">
         <v>331</v>
       </c>
-      <c r="I29" s="261"/>
-      <c r="J29" s="261"/>
-      <c r="K29" s="261"/>
-      <c r="L29" s="261"/>
-      <c r="M29" s="262"/>
+      <c r="I29" s="247"/>
+      <c r="J29" s="247"/>
+      <c r="K29" s="247"/>
+      <c r="L29" s="247"/>
+      <c r="M29" s="248"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="89"/>
@@ -3130,11 +3130,11 @@
     </row>
     <row r="31" spans="2:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B31" s="89"/>
-      <c r="C31" s="281" t="s">
+      <c r="C31" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="281"/>
-      <c r="E31" s="282"/>
+      <c r="D31" s="163"/>
+      <c r="E31" s="164"/>
       <c r="F31" s="11" t="s">
         <v>16</v>
       </c>
@@ -3295,12 +3295,12 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="253" t="s">
+      <c r="H40" s="165" t="s">
         <v>310</v>
       </c>
-      <c r="I40" s="254"/>
-      <c r="J40" s="254"/>
-      <c r="K40" s="255"/>
+      <c r="I40" s="166"/>
+      <c r="J40" s="166"/>
+      <c r="K40" s="167"/>
       <c r="L40" s="20"/>
       <c r="M40" s="79"/>
     </row>
@@ -3313,12 +3313,12 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
-      <c r="H41" s="253" t="s">
+      <c r="H41" s="165" t="s">
         <v>311</v>
       </c>
-      <c r="I41" s="254"/>
-      <c r="J41" s="254"/>
-      <c r="K41" s="255"/>
+      <c r="I41" s="166"/>
+      <c r="J41" s="166"/>
+      <c r="K41" s="167"/>
       <c r="L41" s="20"/>
       <c r="M41" s="79"/>
     </row>
@@ -3331,12 +3331,12 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
-      <c r="H42" s="253" t="s">
+      <c r="H42" s="165" t="s">
         <v>312</v>
       </c>
-      <c r="I42" s="254"/>
-      <c r="J42" s="254"/>
-      <c r="K42" s="255"/>
+      <c r="I42" s="166"/>
+      <c r="J42" s="166"/>
+      <c r="K42" s="167"/>
       <c r="L42" s="20"/>
       <c r="M42" s="79"/>
     </row>
@@ -3349,12 +3349,12 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
-      <c r="H43" s="253" t="s">
+      <c r="H43" s="165" t="s">
         <v>325</v>
       </c>
-      <c r="I43" s="254"/>
-      <c r="J43" s="254"/>
-      <c r="K43" s="255"/>
+      <c r="I43" s="166"/>
+      <c r="J43" s="166"/>
+      <c r="K43" s="167"/>
       <c r="L43" s="20"/>
       <c r="M43" s="79"/>
     </row>
@@ -3412,12 +3412,12 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
-      <c r="H47" s="253" t="s">
+      <c r="H47" s="165" t="s">
         <v>310</v>
       </c>
-      <c r="I47" s="254"/>
-      <c r="J47" s="254"/>
-      <c r="K47" s="255"/>
+      <c r="I47" s="166"/>
+      <c r="J47" s="166"/>
+      <c r="K47" s="167"/>
       <c r="L47" s="20"/>
       <c r="M47" s="79"/>
     </row>
@@ -3430,12 +3430,12 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
-      <c r="H48" s="253" t="s">
+      <c r="H48" s="165" t="s">
         <v>311</v>
       </c>
-      <c r="I48" s="254"/>
-      <c r="J48" s="254"/>
-      <c r="K48" s="255"/>
+      <c r="I48" s="166"/>
+      <c r="J48" s="166"/>
+      <c r="K48" s="167"/>
       <c r="L48" s="20"/>
       <c r="M48" s="79"/>
     </row>
@@ -3448,12 +3448,12 @@
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
-      <c r="H49" s="250" t="s">
+      <c r="H49" s="239" t="s">
         <v>313</v>
       </c>
-      <c r="I49" s="251"/>
-      <c r="J49" s="251"/>
-      <c r="K49" s="252"/>
+      <c r="I49" s="240"/>
+      <c r="J49" s="240"/>
+      <c r="K49" s="241"/>
       <c r="L49" s="149"/>
       <c r="M49" s="79"/>
     </row>
@@ -3466,12 +3466,12 @@
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
-      <c r="H50" s="161" t="s">
+      <c r="H50" s="268" t="s">
         <v>333</v>
       </c>
-      <c r="I50" s="161"/>
-      <c r="J50" s="161"/>
-      <c r="K50" s="161"/>
+      <c r="I50" s="268"/>
+      <c r="J50" s="268"/>
+      <c r="K50" s="268"/>
       <c r="L50" s="158"/>
       <c r="M50" s="138"/>
       <c r="N50" s="138"/>
@@ -3520,12 +3520,12 @@
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
-      <c r="H53" s="253" t="s">
+      <c r="H53" s="165" t="s">
         <v>310</v>
       </c>
-      <c r="I53" s="254"/>
-      <c r="J53" s="254"/>
-      <c r="K53" s="255"/>
+      <c r="I53" s="166"/>
+      <c r="J53" s="166"/>
+      <c r="K53" s="167"/>
       <c r="L53" s="20"/>
       <c r="M53" s="79"/>
     </row>
@@ -3538,12 +3538,12 @@
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
-      <c r="H54" s="170" t="s">
+      <c r="H54" s="274" t="s">
         <v>311</v>
       </c>
-      <c r="I54" s="171"/>
-      <c r="J54" s="171"/>
-      <c r="K54" s="172"/>
+      <c r="I54" s="275"/>
+      <c r="J54" s="275"/>
+      <c r="K54" s="276"/>
       <c r="L54" s="20"/>
       <c r="M54" s="79"/>
     </row>
@@ -3556,12 +3556,12 @@
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
-      <c r="H55" s="161" t="s">
+      <c r="H55" s="268" t="s">
         <v>314</v>
       </c>
-      <c r="I55" s="161"/>
-      <c r="J55" s="161"/>
-      <c r="K55" s="161"/>
+      <c r="I55" s="268"/>
+      <c r="J55" s="268"/>
+      <c r="K55" s="268"/>
       <c r="L55" s="158"/>
       <c r="M55" s="138"/>
       <c r="N55" s="138"/>
@@ -3578,12 +3578,12 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
-      <c r="H56" s="162" t="s">
+      <c r="H56" s="269" t="s">
         <v>315</v>
       </c>
-      <c r="I56" s="163"/>
-      <c r="J56" s="163"/>
-      <c r="K56" s="164"/>
+      <c r="I56" s="270"/>
+      <c r="J56" s="270"/>
+      <c r="K56" s="271"/>
       <c r="L56" s="158"/>
       <c r="M56" s="138"/>
       <c r="N56" s="138"/>
@@ -3863,11 +3863,11 @@
       <c r="F73" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="G73" s="203" t="s">
+      <c r="G73" s="186" t="s">
         <v>51</v>
       </c>
-      <c r="H73" s="204"/>
-      <c r="I73" s="205"/>
+      <c r="H73" s="187"/>
+      <c r="I73" s="188"/>
       <c r="J73" s="90"/>
       <c r="K73" s="90"/>
       <c r="L73" s="90"/>
@@ -3887,11 +3887,11 @@
       <c r="F74" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="G74" s="200" t="s">
+      <c r="G74" s="280" t="s">
         <v>340</v>
       </c>
-      <c r="H74" s="201"/>
-      <c r="I74" s="202"/>
+      <c r="H74" s="281"/>
+      <c r="I74" s="282"/>
       <c r="J74" s="90"/>
       <c r="K74" s="90"/>
       <c r="L74" s="90"/>
@@ -4023,10 +4023,10 @@
       <c r="B83" s="15"/>
       <c r="C83" s="79"/>
       <c r="D83" s="80"/>
-      <c r="E83" s="267" t="s">
+      <c r="E83" s="168" t="s">
         <v>265</v>
       </c>
-      <c r="F83" s="267"/>
+      <c r="F83" s="168"/>
       <c r="I83" s="80"/>
       <c r="J83" s="80"/>
       <c r="K83" s="80"/>
@@ -4112,17 +4112,17 @@
     </row>
     <row r="88" spans="2:13" s="97" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="58"/>
-      <c r="C88" s="168" t="s">
+      <c r="C88" s="273" t="s">
         <v>268</v>
       </c>
-      <c r="D88" s="168"/>
-      <c r="E88" s="168"/>
-      <c r="F88" s="168"/>
-      <c r="G88" s="168"/>
-      <c r="H88" s="168"/>
-      <c r="I88" s="168"/>
-      <c r="J88" s="168"/>
-      <c r="K88" s="168"/>
+      <c r="D88" s="273"/>
+      <c r="E88" s="273"/>
+      <c r="F88" s="273"/>
+      <c r="G88" s="273"/>
+      <c r="H88" s="273"/>
+      <c r="I88" s="273"/>
+      <c r="J88" s="273"/>
+      <c r="K88" s="273"/>
       <c r="L88" s="147"/>
       <c r="M88" s="80"/>
     </row>
@@ -4289,10 +4289,10 @@
       </c>
       <c r="D99" s="103"/>
       <c r="E99" s="67"/>
-      <c r="F99" s="195" t="s">
+      <c r="F99" s="278" t="s">
         <v>280</v>
       </c>
-      <c r="G99" s="196"/>
+      <c r="G99" s="279"/>
       <c r="H99" s="107"/>
       <c r="I99" s="79"/>
       <c r="J99" s="79"/>
@@ -4472,13 +4472,13 @@
     </row>
     <row r="111" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" s="58"/>
-      <c r="C111" s="241" t="s">
+      <c r="C111" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="D111" s="241"/>
-      <c r="E111" s="241"/>
-      <c r="F111" s="241"/>
-      <c r="G111" s="242"/>
+      <c r="D111" s="218"/>
+      <c r="E111" s="218"/>
+      <c r="F111" s="218"/>
+      <c r="G111" s="219"/>
       <c r="H111" s="26"/>
       <c r="I111" s="27"/>
       <c r="J111" s="80"/>
@@ -4493,8 +4493,8 @@
       <c r="E112" s="79"/>
       <c r="F112" s="79"/>
       <c r="G112" s="79"/>
-      <c r="H112" s="243"/>
-      <c r="I112" s="243"/>
+      <c r="H112" s="220"/>
+      <c r="I112" s="220"/>
       <c r="J112" s="80"/>
       <c r="K112" s="80"/>
       <c r="L112" s="152"/>
@@ -4502,13 +4502,13 @@
     </row>
     <row r="113" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" s="58"/>
-      <c r="C113" s="241" t="s">
+      <c r="C113" s="218" t="s">
         <v>75</v>
       </c>
-      <c r="D113" s="241"/>
-      <c r="E113" s="241"/>
-      <c r="F113" s="241"/>
-      <c r="G113" s="242"/>
+      <c r="D113" s="218"/>
+      <c r="E113" s="218"/>
+      <c r="F113" s="218"/>
+      <c r="G113" s="219"/>
       <c r="H113" s="26"/>
       <c r="I113" s="27"/>
       <c r="J113" s="80"/>
@@ -4640,47 +4640,47 @@
     </row>
     <row r="122" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122" s="58"/>
-      <c r="C122" s="244" t="s">
+      <c r="C122" s="221" t="s">
         <v>281</v>
       </c>
-      <c r="D122" s="245"/>
-      <c r="E122" s="245"/>
-      <c r="F122" s="245"/>
-      <c r="G122" s="245"/>
-      <c r="H122" s="245"/>
-      <c r="I122" s="245"/>
-      <c r="J122" s="245"/>
-      <c r="K122" s="245"/>
-      <c r="L122" s="245"/>
-      <c r="M122" s="246"/>
+      <c r="D122" s="222"/>
+      <c r="E122" s="222"/>
+      <c r="F122" s="222"/>
+      <c r="G122" s="222"/>
+      <c r="H122" s="222"/>
+      <c r="I122" s="222"/>
+      <c r="J122" s="222"/>
+      <c r="K122" s="222"/>
+      <c r="L122" s="222"/>
+      <c r="M122" s="223"/>
     </row>
     <row r="123" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="58"/>
-      <c r="C123" s="197"/>
-      <c r="D123" s="198"/>
-      <c r="E123" s="198"/>
-      <c r="F123" s="198"/>
-      <c r="G123" s="198"/>
-      <c r="H123" s="198"/>
-      <c r="I123" s="198"/>
-      <c r="J123" s="198"/>
-      <c r="K123" s="198"/>
-      <c r="L123" s="198"/>
-      <c r="M123" s="199"/>
+      <c r="C123" s="224"/>
+      <c r="D123" s="225"/>
+      <c r="E123" s="225"/>
+      <c r="F123" s="225"/>
+      <c r="G123" s="225"/>
+      <c r="H123" s="225"/>
+      <c r="I123" s="225"/>
+      <c r="J123" s="225"/>
+      <c r="K123" s="225"/>
+      <c r="L123" s="225"/>
+      <c r="M123" s="226"/>
     </row>
     <row r="124" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="58"/>
-      <c r="C124" s="247"/>
-      <c r="D124" s="248"/>
-      <c r="E124" s="248"/>
-      <c r="F124" s="248"/>
-      <c r="G124" s="248"/>
-      <c r="H124" s="248"/>
-      <c r="I124" s="248"/>
-      <c r="J124" s="248"/>
-      <c r="K124" s="248"/>
-      <c r="L124" s="248"/>
-      <c r="M124" s="249"/>
+      <c r="C124" s="227"/>
+      <c r="D124" s="228"/>
+      <c r="E124" s="228"/>
+      <c r="F124" s="228"/>
+      <c r="G124" s="228"/>
+      <c r="H124" s="228"/>
+      <c r="I124" s="228"/>
+      <c r="J124" s="228"/>
+      <c r="K124" s="228"/>
+      <c r="L124" s="228"/>
+      <c r="M124" s="229"/>
     </row>
     <row r="125" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="58"/>
@@ -4714,19 +4714,19 @@
     </row>
     <row r="127" spans="2:13" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="58"/>
-      <c r="C127" s="234" t="s">
+      <c r="C127" s="210" t="s">
         <v>282</v>
       </c>
-      <c r="D127" s="235"/>
-      <c r="E127" s="235"/>
-      <c r="F127" s="235"/>
-      <c r="G127" s="235"/>
-      <c r="H127" s="235"/>
-      <c r="I127" s="235"/>
-      <c r="J127" s="235"/>
-      <c r="K127" s="235"/>
-      <c r="L127" s="235"/>
-      <c r="M127" s="236"/>
+      <c r="D127" s="211"/>
+      <c r="E127" s="211"/>
+      <c r="F127" s="211"/>
+      <c r="G127" s="211"/>
+      <c r="H127" s="211"/>
+      <c r="I127" s="211"/>
+      <c r="J127" s="211"/>
+      <c r="K127" s="211"/>
+      <c r="L127" s="211"/>
+      <c r="M127" s="212"/>
     </row>
     <row r="128" spans="2:13" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="58"/>
@@ -4760,19 +4760,19 @@
     </row>
     <row r="130" spans="2:13" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="58"/>
-      <c r="C130" s="237" t="s">
+      <c r="C130" s="213" t="s">
         <v>283</v>
       </c>
-      <c r="D130" s="238"/>
-      <c r="E130" s="238"/>
-      <c r="F130" s="238"/>
-      <c r="G130" s="238"/>
-      <c r="H130" s="238"/>
-      <c r="I130" s="238"/>
-      <c r="J130" s="238"/>
-      <c r="K130" s="238"/>
-      <c r="L130" s="238"/>
-      <c r="M130" s="239"/>
+      <c r="D130" s="214"/>
+      <c r="E130" s="214"/>
+      <c r="F130" s="214"/>
+      <c r="G130" s="214"/>
+      <c r="H130" s="214"/>
+      <c r="I130" s="214"/>
+      <c r="J130" s="214"/>
+      <c r="K130" s="214"/>
+      <c r="L130" s="214"/>
+      <c r="M130" s="215"/>
     </row>
     <row r="131" spans="2:13" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="58"/>
@@ -4971,19 +4971,19 @@
     </row>
     <row r="144" spans="2:13" ht="87" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="58"/>
-      <c r="C144" s="240" t="s">
+      <c r="C144" s="216" t="s">
         <v>284</v>
       </c>
-      <c r="D144" s="240"/>
-      <c r="E144" s="240"/>
-      <c r="F144" s="240"/>
-      <c r="G144" s="240"/>
-      <c r="H144" s="240"/>
-      <c r="I144" s="240"/>
-      <c r="J144" s="240"/>
-      <c r="K144" s="240"/>
-      <c r="L144" s="240"/>
-      <c r="M144" s="240"/>
+      <c r="D144" s="216"/>
+      <c r="E144" s="216"/>
+      <c r="F144" s="216"/>
+      <c r="G144" s="216"/>
+      <c r="H144" s="216"/>
+      <c r="I144" s="216"/>
+      <c r="J144" s="216"/>
+      <c r="K144" s="216"/>
+      <c r="L144" s="216"/>
+      <c r="M144" s="216"/>
     </row>
     <row r="145" spans="2:13" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="58"/>
@@ -5001,11 +5001,11 @@
     </row>
     <row r="146" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B146" s="18"/>
-      <c r="C146" s="165" t="s">
+      <c r="C146" s="217" t="s">
         <v>91</v>
       </c>
-      <c r="D146" s="165"/>
-      <c r="E146" s="165"/>
+      <c r="D146" s="217"/>
+      <c r="E146" s="217"/>
       <c r="H146" s="106"/>
       <c r="I146" s="18" t="s">
         <v>92</v>
@@ -5029,11 +5029,11 @@
     </row>
     <row r="148" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B148" s="18"/>
-      <c r="C148" s="165" t="s">
+      <c r="C148" s="217" t="s">
         <v>93</v>
       </c>
-      <c r="D148" s="165"/>
-      <c r="E148" s="165"/>
+      <c r="D148" s="217"/>
+      <c r="E148" s="217"/>
       <c r="H148" s="106"/>
       <c r="I148" s="18" t="s">
         <v>94</v>
@@ -5057,11 +5057,11 @@
     </row>
     <row r="150" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B150" s="18"/>
-      <c r="C150" s="165" t="s">
+      <c r="C150" s="217" t="s">
         <v>95</v>
       </c>
-      <c r="D150" s="165"/>
-      <c r="E150" s="165"/>
+      <c r="D150" s="217"/>
+      <c r="E150" s="217"/>
       <c r="H150" s="106"/>
       <c r="I150" s="25"/>
       <c r="J150" s="25"/>
@@ -5083,12 +5083,12 @@
     </row>
     <row r="152" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="18"/>
-      <c r="C152" s="165" t="s">
+      <c r="C152" s="217" t="s">
         <v>96</v>
       </c>
-      <c r="D152" s="165"/>
-      <c r="E152" s="165"/>
-      <c r="F152" s="165"/>
+      <c r="D152" s="217"/>
+      <c r="E152" s="217"/>
+      <c r="F152" s="217"/>
       <c r="H152" s="106"/>
       <c r="I152" s="25"/>
       <c r="J152" s="25"/>
@@ -5111,13 +5111,13 @@
     </row>
     <row r="154" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="18"/>
-      <c r="C154" s="165" t="s">
+      <c r="C154" s="217" t="s">
         <v>97</v>
       </c>
-      <c r="D154" s="165"/>
-      <c r="E154" s="165"/>
-      <c r="F154" s="165"/>
-      <c r="G154" s="166"/>
+      <c r="D154" s="217"/>
+      <c r="E154" s="217"/>
+      <c r="F154" s="217"/>
+      <c r="G154" s="252"/>
       <c r="H154" s="106"/>
       <c r="I154" s="25"/>
     </row>
@@ -5245,19 +5245,19 @@
     </row>
     <row r="163" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="18"/>
-      <c r="C163" s="263" t="s">
+      <c r="C163" s="249" t="s">
         <v>285</v>
       </c>
-      <c r="D163" s="264"/>
-      <c r="E163" s="264"/>
-      <c r="F163" s="264"/>
-      <c r="G163" s="264"/>
-      <c r="H163" s="264"/>
-      <c r="I163" s="264"/>
-      <c r="J163" s="264"/>
-      <c r="K163" s="264"/>
-      <c r="L163" s="264"/>
-      <c r="M163" s="265"/>
+      <c r="D163" s="250"/>
+      <c r="E163" s="250"/>
+      <c r="F163" s="250"/>
+      <c r="G163" s="250"/>
+      <c r="H163" s="250"/>
+      <c r="I163" s="250"/>
+      <c r="J163" s="250"/>
+      <c r="K163" s="250"/>
+      <c r="L163" s="250"/>
+      <c r="M163" s="251"/>
     </row>
     <row r="164" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="18"/>
@@ -5475,12 +5475,12 @@
     </row>
     <row r="180" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B180" s="25"/>
-      <c r="C180" s="165" t="s">
+      <c r="C180" s="217" t="s">
         <v>93</v>
       </c>
-      <c r="D180" s="165"/>
-      <c r="E180" s="165"/>
-      <c r="F180" s="165"/>
+      <c r="D180" s="217"/>
+      <c r="E180" s="217"/>
+      <c r="F180" s="217"/>
       <c r="G180" s="79"/>
       <c r="H180" s="103"/>
       <c r="I180" s="18" t="s">
@@ -5507,13 +5507,13 @@
     </row>
     <row r="182" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B182" s="25"/>
-      <c r="C182" s="165" t="s">
+      <c r="C182" s="217" t="s">
         <v>112</v>
       </c>
-      <c r="D182" s="165"/>
-      <c r="E182" s="165"/>
-      <c r="F182" s="165"/>
-      <c r="G182" s="166"/>
+      <c r="D182" s="217"/>
+      <c r="E182" s="217"/>
+      <c r="F182" s="217"/>
+      <c r="G182" s="252"/>
       <c r="H182" s="103"/>
       <c r="I182" s="25"/>
       <c r="J182" s="25"/>
@@ -5567,13 +5567,13 @@
     </row>
     <row r="186" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B186" s="25"/>
-      <c r="C186" s="165" t="s">
+      <c r="C186" s="217" t="s">
         <v>114</v>
       </c>
-      <c r="D186" s="165"/>
-      <c r="E186" s="165"/>
-      <c r="F186" s="165"/>
-      <c r="G186" s="166"/>
+      <c r="D186" s="217"/>
+      <c r="E186" s="217"/>
+      <c r="F186" s="217"/>
+      <c r="G186" s="252"/>
       <c r="H186" s="103"/>
       <c r="I186" s="25"/>
       <c r="J186" s="25"/>
@@ -5686,79 +5686,79 @@
     </row>
     <row r="194" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="21"/>
-      <c r="C194" s="182" t="s">
+      <c r="C194" s="230" t="s">
         <v>286</v>
       </c>
-      <c r="D194" s="183"/>
-      <c r="E194" s="183"/>
-      <c r="F194" s="183"/>
-      <c r="G194" s="183"/>
-      <c r="H194" s="183"/>
-      <c r="I194" s="183"/>
-      <c r="J194" s="183"/>
-      <c r="K194" s="183"/>
-      <c r="L194" s="183"/>
-      <c r="M194" s="184"/>
+      <c r="D194" s="231"/>
+      <c r="E194" s="231"/>
+      <c r="F194" s="231"/>
+      <c r="G194" s="231"/>
+      <c r="H194" s="231"/>
+      <c r="I194" s="231"/>
+      <c r="J194" s="231"/>
+      <c r="K194" s="231"/>
+      <c r="L194" s="231"/>
+      <c r="M194" s="232"/>
       <c r="N194" s="21"/>
     </row>
     <row r="195" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="21"/>
-      <c r="C195" s="185"/>
-      <c r="D195" s="186"/>
-      <c r="E195" s="186"/>
-      <c r="F195" s="186"/>
-      <c r="G195" s="186"/>
-      <c r="H195" s="186"/>
-      <c r="I195" s="186"/>
-      <c r="J195" s="186"/>
-      <c r="K195" s="186"/>
-      <c r="L195" s="186"/>
-      <c r="M195" s="187"/>
+      <c r="C195" s="233"/>
+      <c r="D195" s="234"/>
+      <c r="E195" s="234"/>
+      <c r="F195" s="234"/>
+      <c r="G195" s="234"/>
+      <c r="H195" s="234"/>
+      <c r="I195" s="234"/>
+      <c r="J195" s="234"/>
+      <c r="K195" s="234"/>
+      <c r="L195" s="234"/>
+      <c r="M195" s="235"/>
       <c r="N195" s="2"/>
     </row>
     <row r="196" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="21"/>
-      <c r="C196" s="185"/>
-      <c r="D196" s="186"/>
-      <c r="E196" s="186"/>
-      <c r="F196" s="186"/>
-      <c r="G196" s="186"/>
-      <c r="H196" s="186"/>
-      <c r="I196" s="186"/>
-      <c r="J196" s="186"/>
-      <c r="K196" s="186"/>
-      <c r="L196" s="186"/>
-      <c r="M196" s="187"/>
+      <c r="C196" s="233"/>
+      <c r="D196" s="234"/>
+      <c r="E196" s="234"/>
+      <c r="F196" s="234"/>
+      <c r="G196" s="234"/>
+      <c r="H196" s="234"/>
+      <c r="I196" s="234"/>
+      <c r="J196" s="234"/>
+      <c r="K196" s="234"/>
+      <c r="L196" s="234"/>
+      <c r="M196" s="235"/>
       <c r="N196" s="2"/>
     </row>
     <row r="197" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="21"/>
-      <c r="C197" s="185"/>
-      <c r="D197" s="186"/>
-      <c r="E197" s="186"/>
-      <c r="F197" s="186"/>
-      <c r="G197" s="186"/>
-      <c r="H197" s="186"/>
-      <c r="I197" s="186"/>
-      <c r="J197" s="186"/>
-      <c r="K197" s="186"/>
-      <c r="L197" s="186"/>
-      <c r="M197" s="187"/>
+      <c r="C197" s="233"/>
+      <c r="D197" s="234"/>
+      <c r="E197" s="234"/>
+      <c r="F197" s="234"/>
+      <c r="G197" s="234"/>
+      <c r="H197" s="234"/>
+      <c r="I197" s="234"/>
+      <c r="J197" s="234"/>
+      <c r="K197" s="234"/>
+      <c r="L197" s="234"/>
+      <c r="M197" s="235"/>
       <c r="N197" s="2"/>
     </row>
     <row r="198" spans="2:14" ht="99.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="21"/>
-      <c r="C198" s="188"/>
-      <c r="D198" s="189"/>
-      <c r="E198" s="189"/>
-      <c r="F198" s="189"/>
-      <c r="G198" s="189"/>
-      <c r="H198" s="189"/>
-      <c r="I198" s="189"/>
-      <c r="J198" s="189"/>
-      <c r="K198" s="189"/>
-      <c r="L198" s="189"/>
-      <c r="M198" s="190"/>
+      <c r="C198" s="236"/>
+      <c r="D198" s="237"/>
+      <c r="E198" s="237"/>
+      <c r="F198" s="237"/>
+      <c r="G198" s="237"/>
+      <c r="H198" s="237"/>
+      <c r="I198" s="237"/>
+      <c r="J198" s="237"/>
+      <c r="K198" s="237"/>
+      <c r="L198" s="237"/>
+      <c r="M198" s="238"/>
       <c r="N198" s="2"/>
     </row>
     <row r="199" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5795,79 +5795,79 @@
     </row>
     <row r="201" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="21"/>
-      <c r="C201" s="182" t="s">
+      <c r="C201" s="230" t="s">
         <v>287</v>
       </c>
-      <c r="D201" s="183"/>
-      <c r="E201" s="183"/>
-      <c r="F201" s="183"/>
-      <c r="G201" s="183"/>
-      <c r="H201" s="183"/>
-      <c r="I201" s="183"/>
-      <c r="J201" s="183"/>
-      <c r="K201" s="183"/>
-      <c r="L201" s="183"/>
-      <c r="M201" s="184"/>
+      <c r="D201" s="231"/>
+      <c r="E201" s="231"/>
+      <c r="F201" s="231"/>
+      <c r="G201" s="231"/>
+      <c r="H201" s="231"/>
+      <c r="I201" s="231"/>
+      <c r="J201" s="231"/>
+      <c r="K201" s="231"/>
+      <c r="L201" s="231"/>
+      <c r="M201" s="232"/>
       <c r="N201" s="34"/>
     </row>
     <row r="202" spans="2:14" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="21"/>
-      <c r="C202" s="185"/>
-      <c r="D202" s="186"/>
-      <c r="E202" s="186"/>
-      <c r="F202" s="186"/>
-      <c r="G202" s="186"/>
-      <c r="H202" s="186"/>
-      <c r="I202" s="186"/>
-      <c r="J202" s="186"/>
-      <c r="K202" s="186"/>
-      <c r="L202" s="186"/>
-      <c r="M202" s="187"/>
+      <c r="C202" s="233"/>
+      <c r="D202" s="234"/>
+      <c r="E202" s="234"/>
+      <c r="F202" s="234"/>
+      <c r="G202" s="234"/>
+      <c r="H202" s="234"/>
+      <c r="I202" s="234"/>
+      <c r="J202" s="234"/>
+      <c r="K202" s="234"/>
+      <c r="L202" s="234"/>
+      <c r="M202" s="235"/>
       <c r="N202" s="2"/>
     </row>
     <row r="203" spans="2:14" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="21"/>
-      <c r="C203" s="185"/>
-      <c r="D203" s="186"/>
-      <c r="E203" s="186"/>
-      <c r="F203" s="186"/>
-      <c r="G203" s="186"/>
-      <c r="H203" s="186"/>
-      <c r="I203" s="186"/>
-      <c r="J203" s="186"/>
-      <c r="K203" s="186"/>
-      <c r="L203" s="186"/>
-      <c r="M203" s="187"/>
+      <c r="C203" s="233"/>
+      <c r="D203" s="234"/>
+      <c r="E203" s="234"/>
+      <c r="F203" s="234"/>
+      <c r="G203" s="234"/>
+      <c r="H203" s="234"/>
+      <c r="I203" s="234"/>
+      <c r="J203" s="234"/>
+      <c r="K203" s="234"/>
+      <c r="L203" s="234"/>
+      <c r="M203" s="235"/>
       <c r="N203" s="2"/>
     </row>
     <row r="204" spans="2:14" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="21"/>
-      <c r="C204" s="185"/>
-      <c r="D204" s="186"/>
-      <c r="E204" s="186"/>
-      <c r="F204" s="186"/>
-      <c r="G204" s="186"/>
-      <c r="H204" s="186"/>
-      <c r="I204" s="186"/>
-      <c r="J204" s="186"/>
-      <c r="K204" s="186"/>
-      <c r="L204" s="186"/>
-      <c r="M204" s="187"/>
+      <c r="C204" s="233"/>
+      <c r="D204" s="234"/>
+      <c r="E204" s="234"/>
+      <c r="F204" s="234"/>
+      <c r="G204" s="234"/>
+      <c r="H204" s="234"/>
+      <c r="I204" s="234"/>
+      <c r="J204" s="234"/>
+      <c r="K204" s="234"/>
+      <c r="L204" s="234"/>
+      <c r="M204" s="235"/>
       <c r="N204" s="2"/>
     </row>
     <row r="205" spans="2:14" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="21"/>
-      <c r="C205" s="188"/>
-      <c r="D205" s="189"/>
-      <c r="E205" s="189"/>
-      <c r="F205" s="189"/>
-      <c r="G205" s="189"/>
-      <c r="H205" s="189"/>
-      <c r="I205" s="189"/>
-      <c r="J205" s="189"/>
-      <c r="K205" s="189"/>
-      <c r="L205" s="189"/>
-      <c r="M205" s="190"/>
+      <c r="C205" s="236"/>
+      <c r="D205" s="237"/>
+      <c r="E205" s="237"/>
+      <c r="F205" s="237"/>
+      <c r="G205" s="237"/>
+      <c r="H205" s="237"/>
+      <c r="I205" s="237"/>
+      <c r="J205" s="237"/>
+      <c r="K205" s="237"/>
+      <c r="L205" s="237"/>
+      <c r="M205" s="238"/>
       <c r="N205" s="2"/>
     </row>
     <row r="206" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6014,49 +6014,49 @@
     </row>
     <row r="215" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B215" s="18"/>
-      <c r="C215" s="225" t="s">
+      <c r="C215" s="201" t="s">
         <v>292</v>
       </c>
-      <c r="D215" s="226"/>
-      <c r="E215" s="226"/>
-      <c r="F215" s="226"/>
-      <c r="G215" s="226"/>
-      <c r="H215" s="226"/>
-      <c r="I215" s="226"/>
-      <c r="J215" s="226"/>
-      <c r="K215" s="226"/>
-      <c r="L215" s="226"/>
-      <c r="M215" s="227"/>
+      <c r="D215" s="202"/>
+      <c r="E215" s="202"/>
+      <c r="F215" s="202"/>
+      <c r="G215" s="202"/>
+      <c r="H215" s="202"/>
+      <c r="I215" s="202"/>
+      <c r="J215" s="202"/>
+      <c r="K215" s="202"/>
+      <c r="L215" s="202"/>
+      <c r="M215" s="203"/>
       <c r="N215" s="34"/>
     </row>
     <row r="216" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B216" s="18"/>
-      <c r="C216" s="228"/>
-      <c r="D216" s="229"/>
-      <c r="E216" s="229"/>
-      <c r="F216" s="229"/>
-      <c r="G216" s="229"/>
-      <c r="H216" s="229"/>
-      <c r="I216" s="229"/>
-      <c r="J216" s="229"/>
-      <c r="K216" s="229"/>
-      <c r="L216" s="229"/>
-      <c r="M216" s="230"/>
+      <c r="C216" s="204"/>
+      <c r="D216" s="205"/>
+      <c r="E216" s="205"/>
+      <c r="F216" s="205"/>
+      <c r="G216" s="205"/>
+      <c r="H216" s="205"/>
+      <c r="I216" s="205"/>
+      <c r="J216" s="205"/>
+      <c r="K216" s="205"/>
+      <c r="L216" s="205"/>
+      <c r="M216" s="206"/>
       <c r="N216" s="60"/>
     </row>
     <row r="217" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B217" s="18"/>
-      <c r="C217" s="231"/>
-      <c r="D217" s="232"/>
-      <c r="E217" s="232"/>
-      <c r="F217" s="232"/>
-      <c r="G217" s="232"/>
-      <c r="H217" s="232"/>
-      <c r="I217" s="232"/>
-      <c r="J217" s="232"/>
-      <c r="K217" s="232"/>
-      <c r="L217" s="232"/>
-      <c r="M217" s="233"/>
+      <c r="C217" s="207"/>
+      <c r="D217" s="208"/>
+      <c r="E217" s="208"/>
+      <c r="F217" s="208"/>
+      <c r="G217" s="208"/>
+      <c r="H217" s="208"/>
+      <c r="I217" s="208"/>
+      <c r="J217" s="208"/>
+      <c r="K217" s="208"/>
+      <c r="L217" s="208"/>
+      <c r="M217" s="209"/>
       <c r="N217" s="60"/>
     </row>
     <row r="218" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
@@ -6091,10 +6091,10 @@
     </row>
     <row r="220" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B220" s="18"/>
-      <c r="C220" s="165" t="s">
+      <c r="C220" s="217" t="s">
         <v>122</v>
       </c>
-      <c r="D220" s="165"/>
+      <c r="D220" s="217"/>
       <c r="E220" s="82"/>
       <c r="F220" s="79"/>
       <c r="G220" s="13"/>
@@ -6219,19 +6219,19 @@
     </row>
     <row r="228" spans="2:15" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228" s="18"/>
-      <c r="C228" s="197" t="s">
+      <c r="C228" s="224" t="s">
         <v>291</v>
       </c>
-      <c r="D228" s="198"/>
-      <c r="E228" s="198"/>
-      <c r="F228" s="198"/>
-      <c r="G228" s="198"/>
-      <c r="H228" s="198"/>
-      <c r="I228" s="198"/>
-      <c r="J228" s="198"/>
-      <c r="K228" s="198"/>
-      <c r="L228" s="198"/>
-      <c r="M228" s="199"/>
+      <c r="D228" s="225"/>
+      <c r="E228" s="225"/>
+      <c r="F228" s="225"/>
+      <c r="G228" s="225"/>
+      <c r="H228" s="225"/>
+      <c r="I228" s="225"/>
+      <c r="J228" s="225"/>
+      <c r="K228" s="225"/>
+      <c r="L228" s="225"/>
+      <c r="M228" s="226"/>
     </row>
     <row r="229" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B229" s="18"/>
@@ -6340,51 +6340,51 @@
     </row>
     <row r="236" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B236" s="18"/>
-      <c r="C236" s="173" t="s">
+      <c r="C236" s="256" t="s">
         <v>129</v>
       </c>
-      <c r="D236" s="174"/>
-      <c r="E236" s="174"/>
-      <c r="F236" s="174"/>
-      <c r="G236" s="174"/>
-      <c r="H236" s="174"/>
-      <c r="I236" s="174"/>
-      <c r="J236" s="174"/>
-      <c r="K236" s="174"/>
-      <c r="L236" s="174"/>
-      <c r="M236" s="175"/>
+      <c r="D236" s="257"/>
+      <c r="E236" s="257"/>
+      <c r="F236" s="257"/>
+      <c r="G236" s="257"/>
+      <c r="H236" s="257"/>
+      <c r="I236" s="257"/>
+      <c r="J236" s="257"/>
+      <c r="K236" s="257"/>
+      <c r="L236" s="257"/>
+      <c r="M236" s="258"/>
       <c r="N236" s="34"/>
       <c r="O236" s="2"/>
     </row>
     <row r="237" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B237" s="18"/>
-      <c r="C237" s="176"/>
-      <c r="D237" s="177"/>
-      <c r="E237" s="177"/>
-      <c r="F237" s="177"/>
-      <c r="G237" s="177"/>
-      <c r="H237" s="177"/>
-      <c r="I237" s="177"/>
-      <c r="J237" s="177"/>
-      <c r="K237" s="177"/>
-      <c r="L237" s="177"/>
-      <c r="M237" s="178"/>
+      <c r="C237" s="259"/>
+      <c r="D237" s="260"/>
+      <c r="E237" s="260"/>
+      <c r="F237" s="260"/>
+      <c r="G237" s="260"/>
+      <c r="H237" s="260"/>
+      <c r="I237" s="260"/>
+      <c r="J237" s="260"/>
+      <c r="K237" s="260"/>
+      <c r="L237" s="260"/>
+      <c r="M237" s="261"/>
       <c r="N237" s="60"/>
       <c r="O237" s="2"/>
     </row>
     <row r="238" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B238" s="18"/>
-      <c r="C238" s="179"/>
-      <c r="D238" s="180"/>
-      <c r="E238" s="180"/>
-      <c r="F238" s="180"/>
-      <c r="G238" s="180"/>
-      <c r="H238" s="180"/>
-      <c r="I238" s="180"/>
-      <c r="J238" s="180"/>
-      <c r="K238" s="180"/>
-      <c r="L238" s="180"/>
-      <c r="M238" s="181"/>
+      <c r="C238" s="262"/>
+      <c r="D238" s="263"/>
+      <c r="E238" s="263"/>
+      <c r="F238" s="263"/>
+      <c r="G238" s="263"/>
+      <c r="H238" s="263"/>
+      <c r="I238" s="263"/>
+      <c r="J238" s="263"/>
+      <c r="K238" s="263"/>
+      <c r="L238" s="263"/>
+      <c r="M238" s="264"/>
       <c r="N238" s="60"/>
       <c r="O238" s="2"/>
     </row>
@@ -6499,35 +6499,35 @@
     </row>
     <row r="246" spans="2:13" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B246" s="18"/>
-      <c r="C246" s="168" t="s">
+      <c r="C246" s="273" t="s">
         <v>269</v>
       </c>
-      <c r="D246" s="168"/>
-      <c r="E246" s="168"/>
-      <c r="F246" s="168"/>
-      <c r="G246" s="168"/>
-      <c r="H246" s="168"/>
-      <c r="I246" s="168"/>
-      <c r="J246" s="168"/>
-      <c r="K246" s="168"/>
-      <c r="L246" s="168"/>
-      <c r="M246" s="168"/>
+      <c r="D246" s="273"/>
+      <c r="E246" s="273"/>
+      <c r="F246" s="273"/>
+      <c r="G246" s="273"/>
+      <c r="H246" s="273"/>
+      <c r="I246" s="273"/>
+      <c r="J246" s="273"/>
+      <c r="K246" s="273"/>
+      <c r="L246" s="273"/>
+      <c r="M246" s="273"/>
     </row>
     <row r="247" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B247" s="18"/>
-      <c r="C247" s="168" t="s">
+      <c r="C247" s="273" t="s">
         <v>133</v>
       </c>
-      <c r="D247" s="168"/>
-      <c r="E247" s="168"/>
-      <c r="F247" s="168"/>
-      <c r="G247" s="168"/>
-      <c r="H247" s="168"/>
-      <c r="I247" s="168"/>
-      <c r="J247" s="168"/>
-      <c r="K247" s="168"/>
-      <c r="L247" s="168"/>
-      <c r="M247" s="168"/>
+      <c r="D247" s="273"/>
+      <c r="E247" s="273"/>
+      <c r="F247" s="273"/>
+      <c r="G247" s="273"/>
+      <c r="H247" s="273"/>
+      <c r="I247" s="273"/>
+      <c r="J247" s="273"/>
+      <c r="K247" s="273"/>
+      <c r="L247" s="273"/>
+      <c r="M247" s="273"/>
     </row>
     <row r="248" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B248" s="18"/>
@@ -6733,83 +6733,83 @@
     </row>
     <row r="261" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B261" s="18"/>
-      <c r="C261" s="182" t="s">
+      <c r="C261" s="230" t="s">
         <v>304</v>
       </c>
-      <c r="D261" s="183"/>
-      <c r="E261" s="183"/>
-      <c r="F261" s="183"/>
-      <c r="G261" s="183"/>
-      <c r="H261" s="183"/>
-      <c r="I261" s="183"/>
-      <c r="J261" s="183"/>
-      <c r="K261" s="183"/>
-      <c r="L261" s="183"/>
-      <c r="M261" s="184"/>
+      <c r="D261" s="231"/>
+      <c r="E261" s="231"/>
+      <c r="F261" s="231"/>
+      <c r="G261" s="231"/>
+      <c r="H261" s="231"/>
+      <c r="I261" s="231"/>
+      <c r="J261" s="231"/>
+      <c r="K261" s="231"/>
+      <c r="L261" s="231"/>
+      <c r="M261" s="232"/>
       <c r="N261" s="34"/>
       <c r="O261" s="2"/>
     </row>
     <row r="262" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B262" s="18"/>
-      <c r="C262" s="185"/>
-      <c r="D262" s="186"/>
-      <c r="E262" s="186"/>
-      <c r="F262" s="186"/>
-      <c r="G262" s="186"/>
-      <c r="H262" s="186"/>
-      <c r="I262" s="186"/>
-      <c r="J262" s="186"/>
-      <c r="K262" s="186"/>
-      <c r="L262" s="186"/>
-      <c r="M262" s="187"/>
+      <c r="C262" s="233"/>
+      <c r="D262" s="234"/>
+      <c r="E262" s="234"/>
+      <c r="F262" s="234"/>
+      <c r="G262" s="234"/>
+      <c r="H262" s="234"/>
+      <c r="I262" s="234"/>
+      <c r="J262" s="234"/>
+      <c r="K262" s="234"/>
+      <c r="L262" s="234"/>
+      <c r="M262" s="235"/>
       <c r="N262" s="60"/>
       <c r="O262" s="2"/>
     </row>
     <row r="263" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" s="18"/>
-      <c r="C263" s="185"/>
-      <c r="D263" s="186"/>
-      <c r="E263" s="186"/>
-      <c r="F263" s="186"/>
-      <c r="G263" s="186"/>
-      <c r="H263" s="186"/>
-      <c r="I263" s="186"/>
-      <c r="J263" s="186"/>
-      <c r="K263" s="186"/>
-      <c r="L263" s="186"/>
-      <c r="M263" s="187"/>
+      <c r="C263" s="233"/>
+      <c r="D263" s="234"/>
+      <c r="E263" s="234"/>
+      <c r="F263" s="234"/>
+      <c r="G263" s="234"/>
+      <c r="H263" s="234"/>
+      <c r="I263" s="234"/>
+      <c r="J263" s="234"/>
+      <c r="K263" s="234"/>
+      <c r="L263" s="234"/>
+      <c r="M263" s="235"/>
       <c r="N263" s="60"/>
       <c r="O263" s="2"/>
     </row>
     <row r="264" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B264" s="18"/>
-      <c r="C264" s="185"/>
-      <c r="D264" s="186"/>
-      <c r="E264" s="186"/>
-      <c r="F264" s="186"/>
-      <c r="G264" s="186"/>
-      <c r="H264" s="186"/>
-      <c r="I264" s="186"/>
-      <c r="J264" s="186"/>
-      <c r="K264" s="186"/>
-      <c r="L264" s="186"/>
-      <c r="M264" s="187"/>
+      <c r="C264" s="233"/>
+      <c r="D264" s="234"/>
+      <c r="E264" s="234"/>
+      <c r="F264" s="234"/>
+      <c r="G264" s="234"/>
+      <c r="H264" s="234"/>
+      <c r="I264" s="234"/>
+      <c r="J264" s="234"/>
+      <c r="K264" s="234"/>
+      <c r="L264" s="234"/>
+      <c r="M264" s="235"/>
       <c r="N264" s="60"/>
       <c r="O264" s="2"/>
     </row>
     <row r="265" spans="2:15" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B265" s="18"/>
-      <c r="C265" s="188"/>
-      <c r="D265" s="189"/>
-      <c r="E265" s="189"/>
-      <c r="F265" s="189"/>
-      <c r="G265" s="189"/>
-      <c r="H265" s="189"/>
-      <c r="I265" s="189"/>
-      <c r="J265" s="189"/>
-      <c r="K265" s="189"/>
-      <c r="L265" s="189"/>
-      <c r="M265" s="190"/>
+      <c r="C265" s="236"/>
+      <c r="D265" s="237"/>
+      <c r="E265" s="237"/>
+      <c r="F265" s="237"/>
+      <c r="G265" s="237"/>
+      <c r="H265" s="237"/>
+      <c r="I265" s="237"/>
+      <c r="J265" s="237"/>
+      <c r="K265" s="237"/>
+      <c r="L265" s="237"/>
+      <c r="M265" s="238"/>
       <c r="N265" s="60"/>
       <c r="O265" s="2"/>
     </row>
@@ -6865,28 +6865,28 @@
     </row>
     <row r="269" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B269" s="18"/>
-      <c r="C269" s="169" t="s">
+      <c r="C269" s="183" t="s">
         <v>253</v>
       </c>
-      <c r="D269" s="169"/>
-      <c r="E269" s="192" t="s">
+      <c r="D269" s="183"/>
+      <c r="E269" s="179" t="s">
         <v>141</v>
       </c>
-      <c r="F269" s="193"/>
-      <c r="G269" s="193"/>
-      <c r="H269" s="193"/>
-      <c r="I269" s="193"/>
-      <c r="J269" s="193"/>
-      <c r="K269" s="193"/>
-      <c r="L269" s="193"/>
-      <c r="M269" s="194"/>
+      <c r="F269" s="180"/>
+      <c r="G269" s="180"/>
+      <c r="H269" s="180"/>
+      <c r="I269" s="180"/>
+      <c r="J269" s="180"/>
+      <c r="K269" s="180"/>
+      <c r="L269" s="180"/>
+      <c r="M269" s="181"/>
       <c r="N269" s="34"/>
       <c r="O269" s="2"/>
     </row>
     <row r="270" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B270" s="18"/>
-      <c r="C270" s="167"/>
-      <c r="D270" s="167"/>
+      <c r="C270" s="272"/>
+      <c r="D270" s="272"/>
       <c r="E270" s="71"/>
       <c r="F270" s="73"/>
       <c r="G270" s="73"/>
@@ -6901,8 +6901,8 @@
     </row>
     <row r="271" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B271" s="18"/>
-      <c r="C271" s="167"/>
-      <c r="D271" s="167"/>
+      <c r="C271" s="272"/>
+      <c r="D271" s="272"/>
       <c r="E271" s="71"/>
       <c r="F271" s="73"/>
       <c r="G271" s="73"/>
@@ -6917,8 +6917,8 @@
     </row>
     <row r="272" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B272" s="18"/>
-      <c r="C272" s="167"/>
-      <c r="D272" s="167"/>
+      <c r="C272" s="272"/>
+      <c r="D272" s="272"/>
       <c r="E272" s="71"/>
       <c r="F272" s="73"/>
       <c r="G272" s="73"/>
@@ -6933,8 +6933,8 @@
     </row>
     <row r="273" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B273" s="18"/>
-      <c r="C273" s="167"/>
-      <c r="D273" s="167"/>
+      <c r="C273" s="272"/>
+      <c r="D273" s="272"/>
       <c r="E273" s="71"/>
       <c r="F273" s="73"/>
       <c r="G273" s="73"/>
@@ -6999,83 +6999,83 @@
     </row>
     <row r="277" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B277" s="18"/>
-      <c r="C277" s="191" t="s">
+      <c r="C277" s="277" t="s">
         <v>302</v>
       </c>
-      <c r="D277" s="191"/>
-      <c r="E277" s="191"/>
-      <c r="F277" s="191"/>
-      <c r="G277" s="191"/>
-      <c r="H277" s="191"/>
-      <c r="I277" s="191"/>
-      <c r="J277" s="191"/>
-      <c r="K277" s="191"/>
-      <c r="L277" s="191"/>
-      <c r="M277" s="191"/>
+      <c r="D277" s="277"/>
+      <c r="E277" s="277"/>
+      <c r="F277" s="277"/>
+      <c r="G277" s="277"/>
+      <c r="H277" s="277"/>
+      <c r="I277" s="277"/>
+      <c r="J277" s="277"/>
+      <c r="K277" s="277"/>
+      <c r="L277" s="277"/>
+      <c r="M277" s="277"/>
       <c r="N277" s="34"/>
       <c r="O277" s="2"/>
     </row>
     <row r="278" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B278" s="18"/>
-      <c r="C278" s="191"/>
-      <c r="D278" s="191"/>
-      <c r="E278" s="191"/>
-      <c r="F278" s="191"/>
-      <c r="G278" s="191"/>
-      <c r="H278" s="191"/>
-      <c r="I278" s="191"/>
-      <c r="J278" s="191"/>
-      <c r="K278" s="191"/>
-      <c r="L278" s="191"/>
-      <c r="M278" s="191"/>
+      <c r="C278" s="277"/>
+      <c r="D278" s="277"/>
+      <c r="E278" s="277"/>
+      <c r="F278" s="277"/>
+      <c r="G278" s="277"/>
+      <c r="H278" s="277"/>
+      <c r="I278" s="277"/>
+      <c r="J278" s="277"/>
+      <c r="K278" s="277"/>
+      <c r="L278" s="277"/>
+      <c r="M278" s="277"/>
       <c r="N278" s="60"/>
       <c r="O278" s="2"/>
     </row>
     <row r="279" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B279" s="18"/>
-      <c r="C279" s="191"/>
-      <c r="D279" s="191"/>
-      <c r="E279" s="191"/>
-      <c r="F279" s="191"/>
-      <c r="G279" s="191"/>
-      <c r="H279" s="191"/>
-      <c r="I279" s="191"/>
-      <c r="J279" s="191"/>
-      <c r="K279" s="191"/>
-      <c r="L279" s="191"/>
-      <c r="M279" s="191"/>
+      <c r="C279" s="277"/>
+      <c r="D279" s="277"/>
+      <c r="E279" s="277"/>
+      <c r="F279" s="277"/>
+      <c r="G279" s="277"/>
+      <c r="H279" s="277"/>
+      <c r="I279" s="277"/>
+      <c r="J279" s="277"/>
+      <c r="K279" s="277"/>
+      <c r="L279" s="277"/>
+      <c r="M279" s="277"/>
       <c r="N279" s="60"/>
       <c r="O279" s="2"/>
     </row>
     <row r="280" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B280" s="18"/>
-      <c r="C280" s="191"/>
-      <c r="D280" s="191"/>
-      <c r="E280" s="191"/>
-      <c r="F280" s="191"/>
-      <c r="G280" s="191"/>
-      <c r="H280" s="191"/>
-      <c r="I280" s="191"/>
-      <c r="J280" s="191"/>
-      <c r="K280" s="191"/>
-      <c r="L280" s="191"/>
-      <c r="M280" s="191"/>
+      <c r="C280" s="277"/>
+      <c r="D280" s="277"/>
+      <c r="E280" s="277"/>
+      <c r="F280" s="277"/>
+      <c r="G280" s="277"/>
+      <c r="H280" s="277"/>
+      <c r="I280" s="277"/>
+      <c r="J280" s="277"/>
+      <c r="K280" s="277"/>
+      <c r="L280" s="277"/>
+      <c r="M280" s="277"/>
       <c r="N280" s="60"/>
       <c r="O280" s="2"/>
     </row>
     <row r="281" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B281" s="18"/>
-      <c r="C281" s="191"/>
-      <c r="D281" s="191"/>
-      <c r="E281" s="191"/>
-      <c r="F281" s="191"/>
-      <c r="G281" s="191"/>
-      <c r="H281" s="191"/>
-      <c r="I281" s="191"/>
-      <c r="J281" s="191"/>
-      <c r="K281" s="191"/>
-      <c r="L281" s="191"/>
-      <c r="M281" s="191"/>
+      <c r="C281" s="277"/>
+      <c r="D281" s="277"/>
+      <c r="E281" s="277"/>
+      <c r="F281" s="277"/>
+      <c r="G281" s="277"/>
+      <c r="H281" s="277"/>
+      <c r="I281" s="277"/>
+      <c r="J281" s="277"/>
+      <c r="K281" s="277"/>
+      <c r="L281" s="277"/>
+      <c r="M281" s="277"/>
       <c r="N281" s="60"/>
       <c r="O281" s="2"/>
     </row>
@@ -7131,12 +7131,12 @@
     </row>
     <row r="285" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B285" s="18"/>
-      <c r="C285" s="165" t="s">
+      <c r="C285" s="217" t="s">
         <v>144</v>
       </c>
-      <c r="D285" s="165"/>
-      <c r="E285" s="165"/>
-      <c r="F285" s="166"/>
+      <c r="D285" s="217"/>
+      <c r="E285" s="217"/>
+      <c r="F285" s="252"/>
       <c r="G285" s="106"/>
       <c r="H285" s="25"/>
       <c r="I285" s="25"/>
@@ -7147,10 +7147,10 @@
     </row>
     <row r="286" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B286" s="18"/>
-      <c r="C286" s="165"/>
-      <c r="D286" s="165"/>
-      <c r="E286" s="165"/>
-      <c r="F286" s="165"/>
+      <c r="C286" s="217"/>
+      <c r="D286" s="217"/>
+      <c r="E286" s="217"/>
+      <c r="F286" s="217"/>
       <c r="G286" s="13"/>
       <c r="H286" s="25"/>
       <c r="I286" s="25"/>
@@ -7161,12 +7161,12 @@
     </row>
     <row r="287" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B287" s="18"/>
-      <c r="C287" s="165" t="s">
+      <c r="C287" s="217" t="s">
         <v>145</v>
       </c>
-      <c r="D287" s="165"/>
-      <c r="E287" s="165"/>
-      <c r="F287" s="166"/>
+      <c r="D287" s="217"/>
+      <c r="E287" s="217"/>
+      <c r="F287" s="252"/>
       <c r="G287" s="106"/>
       <c r="H287" s="18" t="s">
         <v>146</v>
@@ -7179,10 +7179,10 @@
     </row>
     <row r="288" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B288" s="18"/>
-      <c r="C288" s="165"/>
-      <c r="D288" s="165"/>
-      <c r="E288" s="165"/>
-      <c r="F288" s="165"/>
+      <c r="C288" s="217"/>
+      <c r="D288" s="217"/>
+      <c r="E288" s="217"/>
+      <c r="F288" s="217"/>
       <c r="G288" s="13"/>
       <c r="H288" s="25"/>
       <c r="I288" s="25"/>
@@ -7193,12 +7193,12 @@
     </row>
     <row r="289" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B289" s="18"/>
-      <c r="C289" s="165" t="s">
+      <c r="C289" s="217" t="s">
         <v>147</v>
       </c>
-      <c r="D289" s="165"/>
-      <c r="E289" s="165"/>
-      <c r="F289" s="166"/>
+      <c r="D289" s="217"/>
+      <c r="E289" s="217"/>
+      <c r="F289" s="252"/>
       <c r="G289" s="106"/>
       <c r="H289" s="25"/>
       <c r="I289" s="25"/>
@@ -7223,12 +7223,12 @@
     </row>
     <row r="291" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B291" s="18"/>
-      <c r="C291" s="165" t="s">
+      <c r="C291" s="217" t="s">
         <v>148</v>
       </c>
-      <c r="D291" s="165"/>
-      <c r="E291" s="165"/>
-      <c r="F291" s="166"/>
+      <c r="D291" s="217"/>
+      <c r="E291" s="217"/>
+      <c r="F291" s="252"/>
       <c r="G291" s="106"/>
       <c r="H291" s="25"/>
       <c r="I291" s="25"/>
@@ -7253,12 +7253,12 @@
     </row>
     <row r="293" spans="2:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B293" s="18"/>
-      <c r="C293" s="165" t="s">
+      <c r="C293" s="217" t="s">
         <v>149</v>
       </c>
-      <c r="D293" s="165"/>
-      <c r="E293" s="165"/>
-      <c r="F293" s="166"/>
+      <c r="D293" s="217"/>
+      <c r="E293" s="217"/>
+      <c r="F293" s="252"/>
       <c r="G293" s="106"/>
       <c r="H293" s="25"/>
       <c r="I293" s="25"/>
@@ -7361,82 +7361,82 @@
     </row>
     <row r="300" spans="2:15" ht="6.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B300" s="18"/>
-      <c r="C300" s="182" t="s">
+      <c r="C300" s="230" t="s">
         <v>305</v>
       </c>
-      <c r="D300" s="183"/>
-      <c r="E300" s="183"/>
-      <c r="F300" s="183"/>
-      <c r="G300" s="183"/>
-      <c r="H300" s="183"/>
-      <c r="I300" s="183"/>
-      <c r="J300" s="183"/>
-      <c r="K300" s="183"/>
-      <c r="L300" s="183"/>
-      <c r="M300" s="184"/>
+      <c r="D300" s="231"/>
+      <c r="E300" s="231"/>
+      <c r="F300" s="231"/>
+      <c r="G300" s="231"/>
+      <c r="H300" s="231"/>
+      <c r="I300" s="231"/>
+      <c r="J300" s="231"/>
+      <c r="K300" s="231"/>
+      <c r="L300" s="231"/>
+      <c r="M300" s="232"/>
       <c r="N300" s="21"/>
     </row>
     <row r="301" spans="2:15" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B301" s="18"/>
-      <c r="C301" s="185"/>
-      <c r="D301" s="186"/>
-      <c r="E301" s="186"/>
-      <c r="F301" s="186"/>
-      <c r="G301" s="186"/>
-      <c r="H301" s="186"/>
-      <c r="I301" s="186"/>
-      <c r="J301" s="186"/>
-      <c r="K301" s="186"/>
-      <c r="L301" s="186"/>
-      <c r="M301" s="187"/>
+      <c r="C301" s="233"/>
+      <c r="D301" s="234"/>
+      <c r="E301" s="234"/>
+      <c r="F301" s="234"/>
+      <c r="G301" s="234"/>
+      <c r="H301" s="234"/>
+      <c r="I301" s="234"/>
+      <c r="J301" s="234"/>
+      <c r="K301" s="234"/>
+      <c r="L301" s="234"/>
+      <c r="M301" s="235"/>
       <c r="N301" s="60"/>
       <c r="O301" s="2"/>
     </row>
     <row r="302" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="18"/>
-      <c r="C302" s="185"/>
-      <c r="D302" s="186"/>
-      <c r="E302" s="186"/>
-      <c r="F302" s="186"/>
-      <c r="G302" s="186"/>
-      <c r="H302" s="186"/>
-      <c r="I302" s="186"/>
-      <c r="J302" s="186"/>
-      <c r="K302" s="186"/>
-      <c r="L302" s="186"/>
-      <c r="M302" s="187"/>
+      <c r="C302" s="233"/>
+      <c r="D302" s="234"/>
+      <c r="E302" s="234"/>
+      <c r="F302" s="234"/>
+      <c r="G302" s="234"/>
+      <c r="H302" s="234"/>
+      <c r="I302" s="234"/>
+      <c r="J302" s="234"/>
+      <c r="K302" s="234"/>
+      <c r="L302" s="234"/>
+      <c r="M302" s="235"/>
       <c r="N302" s="60"/>
       <c r="O302" s="2"/>
     </row>
     <row r="303" spans="2:15" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B303" s="18"/>
-      <c r="C303" s="185"/>
-      <c r="D303" s="186"/>
-      <c r="E303" s="186"/>
-      <c r="F303" s="186"/>
-      <c r="G303" s="186"/>
-      <c r="H303" s="186"/>
-      <c r="I303" s="186"/>
-      <c r="J303" s="186"/>
-      <c r="K303" s="186"/>
-      <c r="L303" s="186"/>
-      <c r="M303" s="187"/>
+      <c r="C303" s="233"/>
+      <c r="D303" s="234"/>
+      <c r="E303" s="234"/>
+      <c r="F303" s="234"/>
+      <c r="G303" s="234"/>
+      <c r="H303" s="234"/>
+      <c r="I303" s="234"/>
+      <c r="J303" s="234"/>
+      <c r="K303" s="234"/>
+      <c r="L303" s="234"/>
+      <c r="M303" s="235"/>
       <c r="N303" s="60"/>
       <c r="O303" s="2"/>
     </row>
     <row r="304" spans="2:15" ht="119.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B304" s="18"/>
-      <c r="C304" s="188"/>
-      <c r="D304" s="189"/>
-      <c r="E304" s="189"/>
-      <c r="F304" s="189"/>
-      <c r="G304" s="189"/>
-      <c r="H304" s="189"/>
-      <c r="I304" s="189"/>
-      <c r="J304" s="189"/>
-      <c r="K304" s="189"/>
-      <c r="L304" s="189"/>
-      <c r="M304" s="190"/>
+      <c r="C304" s="236"/>
+      <c r="D304" s="237"/>
+      <c r="E304" s="237"/>
+      <c r="F304" s="237"/>
+      <c r="G304" s="237"/>
+      <c r="H304" s="237"/>
+      <c r="I304" s="237"/>
+      <c r="J304" s="237"/>
+      <c r="K304" s="237"/>
+      <c r="L304" s="237"/>
+      <c r="M304" s="238"/>
       <c r="N304" s="60"/>
       <c r="O304" s="2"/>
     </row>
@@ -7475,83 +7475,83 @@
     </row>
     <row r="307" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B307" s="18"/>
-      <c r="C307" s="182" t="s">
+      <c r="C307" s="230" t="s">
         <v>293</v>
       </c>
-      <c r="D307" s="183"/>
-      <c r="E307" s="183"/>
-      <c r="F307" s="183"/>
-      <c r="G307" s="183"/>
-      <c r="H307" s="183"/>
-      <c r="I307" s="183"/>
-      <c r="J307" s="183"/>
-      <c r="K307" s="183"/>
-      <c r="L307" s="183"/>
-      <c r="M307" s="184"/>
+      <c r="D307" s="231"/>
+      <c r="E307" s="231"/>
+      <c r="F307" s="231"/>
+      <c r="G307" s="231"/>
+      <c r="H307" s="231"/>
+      <c r="I307" s="231"/>
+      <c r="J307" s="231"/>
+      <c r="K307" s="231"/>
+      <c r="L307" s="231"/>
+      <c r="M307" s="232"/>
       <c r="N307" s="34"/>
       <c r="O307" s="2"/>
     </row>
     <row r="308" spans="2:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B308" s="18"/>
-      <c r="C308" s="185"/>
-      <c r="D308" s="186"/>
-      <c r="E308" s="186"/>
-      <c r="F308" s="186"/>
-      <c r="G308" s="186"/>
-      <c r="H308" s="186"/>
-      <c r="I308" s="186"/>
-      <c r="J308" s="186"/>
-      <c r="K308" s="186"/>
-      <c r="L308" s="186"/>
-      <c r="M308" s="187"/>
+      <c r="C308" s="233"/>
+      <c r="D308" s="234"/>
+      <c r="E308" s="234"/>
+      <c r="F308" s="234"/>
+      <c r="G308" s="234"/>
+      <c r="H308" s="234"/>
+      <c r="I308" s="234"/>
+      <c r="J308" s="234"/>
+      <c r="K308" s="234"/>
+      <c r="L308" s="234"/>
+      <c r="M308" s="235"/>
       <c r="N308" s="60"/>
       <c r="O308" s="2"/>
     </row>
     <row r="309" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B309" s="18"/>
-      <c r="C309" s="185"/>
-      <c r="D309" s="186"/>
-      <c r="E309" s="186"/>
-      <c r="F309" s="186"/>
-      <c r="G309" s="186"/>
-      <c r="H309" s="186"/>
-      <c r="I309" s="186"/>
-      <c r="J309" s="186"/>
-      <c r="K309" s="186"/>
-      <c r="L309" s="186"/>
-      <c r="M309" s="187"/>
+      <c r="C309" s="233"/>
+      <c r="D309" s="234"/>
+      <c r="E309" s="234"/>
+      <c r="F309" s="234"/>
+      <c r="G309" s="234"/>
+      <c r="H309" s="234"/>
+      <c r="I309" s="234"/>
+      <c r="J309" s="234"/>
+      <c r="K309" s="234"/>
+      <c r="L309" s="234"/>
+      <c r="M309" s="235"/>
       <c r="N309" s="60"/>
       <c r="O309" s="2"/>
     </row>
     <row r="310" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B310" s="18"/>
-      <c r="C310" s="185"/>
-      <c r="D310" s="186"/>
-      <c r="E310" s="186"/>
-      <c r="F310" s="186"/>
-      <c r="G310" s="186"/>
-      <c r="H310" s="186"/>
-      <c r="I310" s="186"/>
-      <c r="J310" s="186"/>
-      <c r="K310" s="186"/>
-      <c r="L310" s="186"/>
-      <c r="M310" s="187"/>
+      <c r="C310" s="233"/>
+      <c r="D310" s="234"/>
+      <c r="E310" s="234"/>
+      <c r="F310" s="234"/>
+      <c r="G310" s="234"/>
+      <c r="H310" s="234"/>
+      <c r="I310" s="234"/>
+      <c r="J310" s="234"/>
+      <c r="K310" s="234"/>
+      <c r="L310" s="234"/>
+      <c r="M310" s="235"/>
       <c r="N310" s="60"/>
       <c r="O310" s="2"/>
     </row>
     <row r="311" spans="2:15" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B311" s="18"/>
-      <c r="C311" s="188"/>
-      <c r="D311" s="189"/>
-      <c r="E311" s="189"/>
-      <c r="F311" s="189"/>
-      <c r="G311" s="189"/>
-      <c r="H311" s="189"/>
-      <c r="I311" s="189"/>
-      <c r="J311" s="189"/>
-      <c r="K311" s="189"/>
-      <c r="L311" s="189"/>
-      <c r="M311" s="190"/>
+      <c r="C311" s="236"/>
+      <c r="D311" s="237"/>
+      <c r="E311" s="237"/>
+      <c r="F311" s="237"/>
+      <c r="G311" s="237"/>
+      <c r="H311" s="237"/>
+      <c r="I311" s="237"/>
+      <c r="J311" s="237"/>
+      <c r="K311" s="237"/>
+      <c r="L311" s="237"/>
+      <c r="M311" s="238"/>
       <c r="N311" s="60"/>
       <c r="O311" s="2"/>
     </row>
@@ -7731,83 +7731,83 @@
     </row>
     <row r="322" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B322" s="18"/>
-      <c r="C322" s="182" t="s">
+      <c r="C322" s="230" t="s">
         <v>294</v>
       </c>
-      <c r="D322" s="183"/>
-      <c r="E322" s="183"/>
-      <c r="F322" s="183"/>
-      <c r="G322" s="183"/>
-      <c r="H322" s="183"/>
-      <c r="I322" s="183"/>
-      <c r="J322" s="183"/>
-      <c r="K322" s="183"/>
-      <c r="L322" s="183"/>
-      <c r="M322" s="184"/>
+      <c r="D322" s="231"/>
+      <c r="E322" s="231"/>
+      <c r="F322" s="231"/>
+      <c r="G322" s="231"/>
+      <c r="H322" s="231"/>
+      <c r="I322" s="231"/>
+      <c r="J322" s="231"/>
+      <c r="K322" s="231"/>
+      <c r="L322" s="231"/>
+      <c r="M322" s="232"/>
       <c r="N322" s="34"/>
       <c r="O322" s="2"/>
     </row>
     <row r="323" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B323" s="18"/>
-      <c r="C323" s="185"/>
-      <c r="D323" s="186"/>
-      <c r="E323" s="186"/>
-      <c r="F323" s="186"/>
-      <c r="G323" s="186"/>
-      <c r="H323" s="186"/>
-      <c r="I323" s="186"/>
-      <c r="J323" s="186"/>
-      <c r="K323" s="186"/>
-      <c r="L323" s="186"/>
-      <c r="M323" s="187"/>
+      <c r="C323" s="233"/>
+      <c r="D323" s="234"/>
+      <c r="E323" s="234"/>
+      <c r="F323" s="234"/>
+      <c r="G323" s="234"/>
+      <c r="H323" s="234"/>
+      <c r="I323" s="234"/>
+      <c r="J323" s="234"/>
+      <c r="K323" s="234"/>
+      <c r="L323" s="234"/>
+      <c r="M323" s="235"/>
       <c r="N323" s="60"/>
       <c r="O323" s="2"/>
     </row>
     <row r="324" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B324" s="18"/>
-      <c r="C324" s="185"/>
-      <c r="D324" s="186"/>
-      <c r="E324" s="186"/>
-      <c r="F324" s="186"/>
-      <c r="G324" s="186"/>
-      <c r="H324" s="186"/>
-      <c r="I324" s="186"/>
-      <c r="J324" s="186"/>
-      <c r="K324" s="186"/>
-      <c r="L324" s="186"/>
-      <c r="M324" s="187"/>
+      <c r="C324" s="233"/>
+      <c r="D324" s="234"/>
+      <c r="E324" s="234"/>
+      <c r="F324" s="234"/>
+      <c r="G324" s="234"/>
+      <c r="H324" s="234"/>
+      <c r="I324" s="234"/>
+      <c r="J324" s="234"/>
+      <c r="K324" s="234"/>
+      <c r="L324" s="234"/>
+      <c r="M324" s="235"/>
       <c r="N324" s="60"/>
       <c r="O324" s="2"/>
     </row>
     <row r="325" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B325" s="18"/>
-      <c r="C325" s="185"/>
-      <c r="D325" s="186"/>
-      <c r="E325" s="186"/>
-      <c r="F325" s="186"/>
-      <c r="G325" s="186"/>
-      <c r="H325" s="186"/>
-      <c r="I325" s="186"/>
-      <c r="J325" s="186"/>
-      <c r="K325" s="186"/>
-      <c r="L325" s="186"/>
-      <c r="M325" s="187"/>
+      <c r="C325" s="233"/>
+      <c r="D325" s="234"/>
+      <c r="E325" s="234"/>
+      <c r="F325" s="234"/>
+      <c r="G325" s="234"/>
+      <c r="H325" s="234"/>
+      <c r="I325" s="234"/>
+      <c r="J325" s="234"/>
+      <c r="K325" s="234"/>
+      <c r="L325" s="234"/>
+      <c r="M325" s="235"/>
       <c r="N325" s="60"/>
       <c r="O325" s="2"/>
     </row>
     <row r="326" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B326" s="18"/>
-      <c r="C326" s="188"/>
-      <c r="D326" s="189"/>
-      <c r="E326" s="189"/>
-      <c r="F326" s="189"/>
-      <c r="G326" s="189"/>
-      <c r="H326" s="189"/>
-      <c r="I326" s="189"/>
-      <c r="J326" s="189"/>
-      <c r="K326" s="189"/>
-      <c r="L326" s="189"/>
-      <c r="M326" s="190"/>
+      <c r="C326" s="236"/>
+      <c r="D326" s="237"/>
+      <c r="E326" s="237"/>
+      <c r="F326" s="237"/>
+      <c r="G326" s="237"/>
+      <c r="H326" s="237"/>
+      <c r="I326" s="237"/>
+      <c r="J326" s="237"/>
+      <c r="K326" s="237"/>
+      <c r="L326" s="237"/>
+      <c r="M326" s="238"/>
       <c r="N326" s="60"/>
       <c r="O326" s="2"/>
     </row>
@@ -7829,19 +7829,19 @@
     </row>
     <row r="328" spans="2:15" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B328" s="18"/>
-      <c r="C328" s="210" t="s">
+      <c r="C328" s="255" t="s">
         <v>156</v>
       </c>
-      <c r="D328" s="210"/>
-      <c r="E328" s="210"/>
-      <c r="F328" s="210"/>
-      <c r="G328" s="210"/>
-      <c r="H328" s="210"/>
-      <c r="I328" s="210"/>
-      <c r="J328" s="210"/>
-      <c r="K328" s="210"/>
-      <c r="L328" s="210"/>
-      <c r="M328" s="210"/>
+      <c r="D328" s="255"/>
+      <c r="E328" s="255"/>
+      <c r="F328" s="255"/>
+      <c r="G328" s="255"/>
+      <c r="H328" s="255"/>
+      <c r="I328" s="255"/>
+      <c r="J328" s="255"/>
+      <c r="K328" s="255"/>
+      <c r="L328" s="255"/>
+      <c r="M328" s="255"/>
       <c r="N328" s="20"/>
       <c r="O328" s="2"/>
     </row>
@@ -7956,79 +7956,79 @@
     </row>
     <row r="336" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B336" s="18"/>
-      <c r="C336" s="173" t="s">
+      <c r="C336" s="256" t="s">
         <v>252</v>
       </c>
-      <c r="D336" s="174"/>
-      <c r="E336" s="174"/>
-      <c r="F336" s="174"/>
-      <c r="G336" s="174"/>
-      <c r="H336" s="174"/>
-      <c r="I336" s="174"/>
-      <c r="J336" s="174"/>
-      <c r="K336" s="174"/>
-      <c r="L336" s="174"/>
-      <c r="M336" s="175"/>
+      <c r="D336" s="257"/>
+      <c r="E336" s="257"/>
+      <c r="F336" s="257"/>
+      <c r="G336" s="257"/>
+      <c r="H336" s="257"/>
+      <c r="I336" s="257"/>
+      <c r="J336" s="257"/>
+      <c r="K336" s="257"/>
+      <c r="L336" s="257"/>
+      <c r="M336" s="258"/>
       <c r="N336" s="34"/>
     </row>
     <row r="337" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B337" s="18"/>
-      <c r="C337" s="176"/>
-      <c r="D337" s="177"/>
-      <c r="E337" s="177"/>
-      <c r="F337" s="177"/>
-      <c r="G337" s="177"/>
-      <c r="H337" s="177"/>
-      <c r="I337" s="177"/>
-      <c r="J337" s="177"/>
-      <c r="K337" s="177"/>
-      <c r="L337" s="177"/>
-      <c r="M337" s="178"/>
+      <c r="C337" s="259"/>
+      <c r="D337" s="260"/>
+      <c r="E337" s="260"/>
+      <c r="F337" s="260"/>
+      <c r="G337" s="260"/>
+      <c r="H337" s="260"/>
+      <c r="I337" s="260"/>
+      <c r="J337" s="260"/>
+      <c r="K337" s="260"/>
+      <c r="L337" s="260"/>
+      <c r="M337" s="261"/>
       <c r="N337" s="60"/>
     </row>
     <row r="338" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B338" s="18"/>
-      <c r="C338" s="176"/>
-      <c r="D338" s="177"/>
-      <c r="E338" s="177"/>
-      <c r="F338" s="177"/>
-      <c r="G338" s="177"/>
-      <c r="H338" s="177"/>
-      <c r="I338" s="177"/>
-      <c r="J338" s="177"/>
-      <c r="K338" s="177"/>
-      <c r="L338" s="177"/>
-      <c r="M338" s="178"/>
+      <c r="C338" s="259"/>
+      <c r="D338" s="260"/>
+      <c r="E338" s="260"/>
+      <c r="F338" s="260"/>
+      <c r="G338" s="260"/>
+      <c r="H338" s="260"/>
+      <c r="I338" s="260"/>
+      <c r="J338" s="260"/>
+      <c r="K338" s="260"/>
+      <c r="L338" s="260"/>
+      <c r="M338" s="261"/>
       <c r="N338" s="60"/>
     </row>
     <row r="339" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B339" s="18"/>
-      <c r="C339" s="176"/>
-      <c r="D339" s="177"/>
-      <c r="E339" s="177"/>
-      <c r="F339" s="177"/>
-      <c r="G339" s="177"/>
-      <c r="H339" s="177"/>
-      <c r="I339" s="177"/>
-      <c r="J339" s="177"/>
-      <c r="K339" s="177"/>
-      <c r="L339" s="177"/>
-      <c r="M339" s="178"/>
+      <c r="C339" s="259"/>
+      <c r="D339" s="260"/>
+      <c r="E339" s="260"/>
+      <c r="F339" s="260"/>
+      <c r="G339" s="260"/>
+      <c r="H339" s="260"/>
+      <c r="I339" s="260"/>
+      <c r="J339" s="260"/>
+      <c r="K339" s="260"/>
+      <c r="L339" s="260"/>
+      <c r="M339" s="261"/>
       <c r="N339" s="60"/>
     </row>
     <row r="340" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B340" s="18"/>
-      <c r="C340" s="179"/>
-      <c r="D340" s="180"/>
-      <c r="E340" s="180"/>
-      <c r="F340" s="180"/>
-      <c r="G340" s="180"/>
-      <c r="H340" s="180"/>
-      <c r="I340" s="180"/>
-      <c r="J340" s="180"/>
-      <c r="K340" s="180"/>
-      <c r="L340" s="180"/>
-      <c r="M340" s="181"/>
+      <c r="C340" s="262"/>
+      <c r="D340" s="263"/>
+      <c r="E340" s="263"/>
+      <c r="F340" s="263"/>
+      <c r="G340" s="263"/>
+      <c r="H340" s="263"/>
+      <c r="I340" s="263"/>
+      <c r="J340" s="263"/>
+      <c r="K340" s="263"/>
+      <c r="L340" s="263"/>
+      <c r="M340" s="264"/>
       <c r="N340" s="60"/>
     </row>
     <row r="341" spans="2:14" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8048,19 +8048,19 @@
     </row>
     <row r="342" spans="2:14" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B342" s="18"/>
-      <c r="C342" s="210" t="s">
+      <c r="C342" s="255" t="s">
         <v>251</v>
       </c>
-      <c r="D342" s="210"/>
-      <c r="E342" s="210"/>
-      <c r="F342" s="210"/>
-      <c r="G342" s="210"/>
-      <c r="H342" s="210"/>
-      <c r="I342" s="210"/>
-      <c r="J342" s="210"/>
-      <c r="K342" s="210"/>
-      <c r="L342" s="210"/>
-      <c r="M342" s="210"/>
+      <c r="D342" s="255"/>
+      <c r="E342" s="255"/>
+      <c r="F342" s="255"/>
+      <c r="G342" s="255"/>
+      <c r="H342" s="255"/>
+      <c r="I342" s="255"/>
+      <c r="J342" s="255"/>
+      <c r="K342" s="255"/>
+      <c r="L342" s="255"/>
+      <c r="M342" s="255"/>
       <c r="N342" s="60"/>
     </row>
     <row r="343" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
@@ -8109,12 +8109,12 @@
     </row>
     <row r="346" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B346" s="18"/>
-      <c r="C346" s="207" t="s">
+      <c r="C346" s="254" t="s">
         <v>162</v>
       </c>
-      <c r="D346" s="207"/>
-      <c r="E346" s="207"/>
-      <c r="F346" s="207"/>
+      <c r="D346" s="254"/>
+      <c r="E346" s="254"/>
+      <c r="F346" s="254"/>
       <c r="H346" s="106"/>
       <c r="I346" s="25"/>
       <c r="J346" s="25"/>
@@ -8137,12 +8137,12 @@
     </row>
     <row r="348" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B348" s="18"/>
-      <c r="C348" s="207" t="s">
+      <c r="C348" s="254" t="s">
         <v>163</v>
       </c>
-      <c r="D348" s="207"/>
-      <c r="E348" s="207"/>
-      <c r="F348" s="207"/>
+      <c r="D348" s="254"/>
+      <c r="E348" s="254"/>
+      <c r="F348" s="254"/>
       <c r="H348" s="106"/>
       <c r="I348" s="18" t="s">
         <v>164</v>
@@ -8167,13 +8167,13 @@
     </row>
     <row r="350" spans="2:14" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B350" s="18"/>
-      <c r="C350" s="207" t="s">
+      <c r="C350" s="254" t="s">
         <v>165</v>
       </c>
-      <c r="D350" s="207"/>
-      <c r="E350" s="207"/>
-      <c r="F350" s="207"/>
-      <c r="G350" s="166"/>
+      <c r="D350" s="254"/>
+      <c r="E350" s="254"/>
+      <c r="F350" s="254"/>
+      <c r="G350" s="252"/>
       <c r="H350" s="106"/>
       <c r="I350" s="25"/>
       <c r="J350" s="25"/>
@@ -8196,13 +8196,13 @@
     </row>
     <row r="352" spans="2:14" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B352" s="18"/>
-      <c r="C352" s="207" t="s">
+      <c r="C352" s="254" t="s">
         <v>166</v>
       </c>
-      <c r="D352" s="207"/>
-      <c r="E352" s="207"/>
-      <c r="F352" s="207"/>
-      <c r="G352" s="166"/>
+      <c r="D352" s="254"/>
+      <c r="E352" s="254"/>
+      <c r="F352" s="254"/>
+      <c r="G352" s="252"/>
       <c r="H352" s="106"/>
       <c r="I352" s="25"/>
       <c r="J352" s="25"/>
@@ -8225,13 +8225,13 @@
     </row>
     <row r="354" spans="2:15" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B354" s="18"/>
-      <c r="C354" s="207" t="s">
+      <c r="C354" s="254" t="s">
         <v>167</v>
       </c>
-      <c r="D354" s="207"/>
-      <c r="E354" s="207"/>
-      <c r="F354" s="207"/>
-      <c r="G354" s="166"/>
+      <c r="D354" s="254"/>
+      <c r="E354" s="254"/>
+      <c r="F354" s="254"/>
+      <c r="G354" s="252"/>
       <c r="H354" s="106"/>
       <c r="I354" s="25"/>
       <c r="J354" s="25"/>
@@ -8303,83 +8303,83 @@
     </row>
     <row r="359" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B359" s="18"/>
-      <c r="C359" s="182" t="s">
+      <c r="C359" s="230" t="s">
         <v>295</v>
       </c>
-      <c r="D359" s="183"/>
-      <c r="E359" s="183"/>
-      <c r="F359" s="183"/>
-      <c r="G359" s="183"/>
-      <c r="H359" s="183"/>
-      <c r="I359" s="183"/>
-      <c r="J359" s="183"/>
-      <c r="K359" s="183"/>
-      <c r="L359" s="183"/>
-      <c r="M359" s="184"/>
+      <c r="D359" s="231"/>
+      <c r="E359" s="231"/>
+      <c r="F359" s="231"/>
+      <c r="G359" s="231"/>
+      <c r="H359" s="231"/>
+      <c r="I359" s="231"/>
+      <c r="J359" s="231"/>
+      <c r="K359" s="231"/>
+      <c r="L359" s="231"/>
+      <c r="M359" s="232"/>
       <c r="N359" s="34"/>
       <c r="O359" s="2"/>
     </row>
     <row r="360" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B360" s="18"/>
-      <c r="C360" s="185"/>
-      <c r="D360" s="186"/>
-      <c r="E360" s="186"/>
-      <c r="F360" s="186"/>
-      <c r="G360" s="186"/>
-      <c r="H360" s="186"/>
-      <c r="I360" s="186"/>
-      <c r="J360" s="186"/>
-      <c r="K360" s="186"/>
-      <c r="L360" s="186"/>
-      <c r="M360" s="187"/>
+      <c r="C360" s="233"/>
+      <c r="D360" s="234"/>
+      <c r="E360" s="234"/>
+      <c r="F360" s="234"/>
+      <c r="G360" s="234"/>
+      <c r="H360" s="234"/>
+      <c r="I360" s="234"/>
+      <c r="J360" s="234"/>
+      <c r="K360" s="234"/>
+      <c r="L360" s="234"/>
+      <c r="M360" s="235"/>
       <c r="N360" s="60"/>
       <c r="O360" s="2"/>
     </row>
     <row r="361" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B361" s="18"/>
-      <c r="C361" s="185"/>
-      <c r="D361" s="186"/>
-      <c r="E361" s="186"/>
-      <c r="F361" s="186"/>
-      <c r="G361" s="186"/>
-      <c r="H361" s="186"/>
-      <c r="I361" s="186"/>
-      <c r="J361" s="186"/>
-      <c r="K361" s="186"/>
-      <c r="L361" s="186"/>
-      <c r="M361" s="187"/>
+      <c r="C361" s="233"/>
+      <c r="D361" s="234"/>
+      <c r="E361" s="234"/>
+      <c r="F361" s="234"/>
+      <c r="G361" s="234"/>
+      <c r="H361" s="234"/>
+      <c r="I361" s="234"/>
+      <c r="J361" s="234"/>
+      <c r="K361" s="234"/>
+      <c r="L361" s="234"/>
+      <c r="M361" s="235"/>
       <c r="N361" s="60"/>
       <c r="O361" s="2"/>
     </row>
     <row r="362" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B362" s="18"/>
-      <c r="C362" s="185"/>
-      <c r="D362" s="186"/>
-      <c r="E362" s="186"/>
-      <c r="F362" s="186"/>
-      <c r="G362" s="186"/>
-      <c r="H362" s="186"/>
-      <c r="I362" s="186"/>
-      <c r="J362" s="186"/>
-      <c r="K362" s="186"/>
-      <c r="L362" s="186"/>
-      <c r="M362" s="187"/>
+      <c r="C362" s="233"/>
+      <c r="D362" s="234"/>
+      <c r="E362" s="234"/>
+      <c r="F362" s="234"/>
+      <c r="G362" s="234"/>
+      <c r="H362" s="234"/>
+      <c r="I362" s="234"/>
+      <c r="J362" s="234"/>
+      <c r="K362" s="234"/>
+      <c r="L362" s="234"/>
+      <c r="M362" s="235"/>
       <c r="N362" s="60"/>
       <c r="O362" s="2"/>
     </row>
     <row r="363" spans="2:15" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B363" s="18"/>
-      <c r="C363" s="188"/>
-      <c r="D363" s="189"/>
-      <c r="E363" s="189"/>
-      <c r="F363" s="189"/>
-      <c r="G363" s="189"/>
-      <c r="H363" s="189"/>
-      <c r="I363" s="189"/>
-      <c r="J363" s="189"/>
-      <c r="K363" s="189"/>
-      <c r="L363" s="189"/>
-      <c r="M363" s="190"/>
+      <c r="C363" s="236"/>
+      <c r="D363" s="237"/>
+      <c r="E363" s="237"/>
+      <c r="F363" s="237"/>
+      <c r="G363" s="237"/>
+      <c r="H363" s="237"/>
+      <c r="I363" s="237"/>
+      <c r="J363" s="237"/>
+      <c r="K363" s="237"/>
+      <c r="L363" s="237"/>
+      <c r="M363" s="238"/>
       <c r="N363" s="60"/>
       <c r="O363" s="2"/>
     </row>
@@ -8454,28 +8454,28 @@
     </row>
     <row r="368" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B368" s="18"/>
-      <c r="C368" s="211" t="s">
+      <c r="C368" s="265" t="s">
         <v>253</v>
       </c>
-      <c r="D368" s="212"/>
-      <c r="E368" s="208" t="s">
+      <c r="D368" s="266"/>
+      <c r="E368" s="170" t="s">
         <v>141</v>
       </c>
-      <c r="F368" s="213"/>
-      <c r="G368" s="213"/>
-      <c r="H368" s="213"/>
-      <c r="I368" s="213"/>
-      <c r="J368" s="213"/>
-      <c r="K368" s="213"/>
-      <c r="L368" s="213"/>
-      <c r="M368" s="209"/>
+      <c r="F368" s="267"/>
+      <c r="G368" s="267"/>
+      <c r="H368" s="267"/>
+      <c r="I368" s="267"/>
+      <c r="J368" s="267"/>
+      <c r="K368" s="267"/>
+      <c r="L368" s="267"/>
+      <c r="M368" s="171"/>
       <c r="N368" s="20"/>
       <c r="O368" s="2"/>
     </row>
     <row r="369" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B369" s="18"/>
-      <c r="C369" s="208"/>
-      <c r="D369" s="209"/>
+      <c r="C369" s="170"/>
+      <c r="D369" s="171"/>
       <c r="E369" s="71"/>
       <c r="F369" s="73"/>
       <c r="G369" s="73"/>
@@ -8490,19 +8490,19 @@
     </row>
     <row r="370" spans="2:15" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B370" s="18"/>
-      <c r="C370" s="206" t="s">
+      <c r="C370" s="253" t="s">
         <v>270</v>
       </c>
-      <c r="D370" s="206"/>
-      <c r="E370" s="206"/>
-      <c r="F370" s="206"/>
-      <c r="G370" s="206"/>
-      <c r="H370" s="206"/>
-      <c r="I370" s="206"/>
-      <c r="J370" s="206"/>
-      <c r="K370" s="206"/>
-      <c r="L370" s="206"/>
-      <c r="M370" s="206"/>
+      <c r="D370" s="253"/>
+      <c r="E370" s="253"/>
+      <c r="F370" s="253"/>
+      <c r="G370" s="253"/>
+      <c r="H370" s="253"/>
+      <c r="I370" s="253"/>
+      <c r="J370" s="253"/>
+      <c r="K370" s="253"/>
+      <c r="L370" s="253"/>
+      <c r="M370" s="253"/>
       <c r="N370" s="13"/>
       <c r="O370" s="2"/>
     </row>
@@ -8590,20 +8590,20 @@
       <c r="C376" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="D376" s="266" t="s">
+      <c r="D376" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="E376" s="266"/>
-      <c r="F376" s="267" t="s">
+      <c r="E376" s="169"/>
+      <c r="F376" s="168" t="s">
         <v>174</v>
       </c>
-      <c r="G376" s="267"/>
-      <c r="H376" s="267"/>
-      <c r="I376" s="267" t="s">
+      <c r="G376" s="168"/>
+      <c r="H376" s="168"/>
+      <c r="I376" s="168" t="s">
         <v>175</v>
       </c>
-      <c r="J376" s="267"/>
-      <c r="K376" s="267"/>
+      <c r="J376" s="168"/>
+      <c r="K376" s="168"/>
       <c r="L376" s="22"/>
       <c r="M376" s="22"/>
       <c r="N376" s="18"/>
@@ -8613,14 +8613,14 @@
       <c r="C377" s="75">
         <v>1</v>
       </c>
-      <c r="D377" s="266"/>
-      <c r="E377" s="266"/>
-      <c r="F377" s="267"/>
-      <c r="G377" s="267"/>
-      <c r="H377" s="267"/>
-      <c r="I377" s="267"/>
-      <c r="J377" s="267"/>
-      <c r="K377" s="267"/>
+      <c r="D377" s="169"/>
+      <c r="E377" s="169"/>
+      <c r="F377" s="168"/>
+      <c r="G377" s="168"/>
+      <c r="H377" s="168"/>
+      <c r="I377" s="168"/>
+      <c r="J377" s="168"/>
+      <c r="K377" s="168"/>
       <c r="L377" s="22"/>
       <c r="M377" s="34"/>
       <c r="N377" s="76"/>
@@ -8630,14 +8630,14 @@
       <c r="C378" s="75">
         <v>2</v>
       </c>
-      <c r="D378" s="266"/>
-      <c r="E378" s="266"/>
-      <c r="F378" s="267"/>
-      <c r="G378" s="267"/>
-      <c r="H378" s="267"/>
-      <c r="I378" s="267"/>
-      <c r="J378" s="267"/>
-      <c r="K378" s="267"/>
+      <c r="D378" s="169"/>
+      <c r="E378" s="169"/>
+      <c r="F378" s="168"/>
+      <c r="G378" s="168"/>
+      <c r="H378" s="168"/>
+      <c r="I378" s="168"/>
+      <c r="J378" s="168"/>
+      <c r="K378" s="168"/>
       <c r="L378" s="22"/>
       <c r="M378" s="34"/>
       <c r="N378" s="34"/>
@@ -8647,14 +8647,14 @@
       <c r="C379" s="75">
         <v>3</v>
       </c>
-      <c r="D379" s="266"/>
-      <c r="E379" s="266"/>
-      <c r="F379" s="267"/>
-      <c r="G379" s="267"/>
-      <c r="H379" s="267"/>
-      <c r="I379" s="267"/>
-      <c r="J379" s="267"/>
-      <c r="K379" s="267"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
+      <c r="F379" s="168"/>
+      <c r="G379" s="168"/>
+      <c r="H379" s="168"/>
+      <c r="I379" s="168"/>
+      <c r="J379" s="168"/>
+      <c r="K379" s="168"/>
       <c r="L379" s="22"/>
       <c r="M379" s="34"/>
       <c r="N379" s="34"/>
@@ -8664,14 +8664,14 @@
       <c r="C380" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="D380" s="266"/>
-      <c r="E380" s="266"/>
-      <c r="F380" s="267"/>
-      <c r="G380" s="267"/>
-      <c r="H380" s="267"/>
-      <c r="I380" s="267"/>
-      <c r="J380" s="267"/>
-      <c r="K380" s="267"/>
+      <c r="D380" s="169"/>
+      <c r="E380" s="169"/>
+      <c r="F380" s="168"/>
+      <c r="G380" s="168"/>
+      <c r="H380" s="168"/>
+      <c r="I380" s="168"/>
+      <c r="J380" s="168"/>
+      <c r="K380" s="168"/>
       <c r="L380" s="22"/>
       <c r="M380" s="34"/>
       <c r="N380" s="34"/>
@@ -8681,14 +8681,14 @@
       <c r="C381" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="D381" s="266"/>
-      <c r="E381" s="266"/>
-      <c r="F381" s="267"/>
-      <c r="G381" s="267"/>
-      <c r="H381" s="267"/>
-      <c r="I381" s="267"/>
-      <c r="J381" s="267"/>
-      <c r="K381" s="267"/>
+      <c r="D381" s="169"/>
+      <c r="E381" s="169"/>
+      <c r="F381" s="168"/>
+      <c r="G381" s="168"/>
+      <c r="H381" s="168"/>
+      <c r="I381" s="168"/>
+      <c r="J381" s="168"/>
+      <c r="K381" s="168"/>
       <c r="L381" s="22"/>
       <c r="M381" s="34"/>
       <c r="N381" s="34"/>
@@ -8698,14 +8698,14 @@
       <c r="C382" s="75" t="s">
         <v>179</v>
       </c>
-      <c r="D382" s="266"/>
-      <c r="E382" s="266"/>
-      <c r="F382" s="267"/>
-      <c r="G382" s="267"/>
-      <c r="H382" s="267"/>
-      <c r="I382" s="267"/>
-      <c r="J382" s="267"/>
-      <c r="K382" s="267"/>
+      <c r="D382" s="169"/>
+      <c r="E382" s="169"/>
+      <c r="F382" s="168"/>
+      <c r="G382" s="168"/>
+      <c r="H382" s="168"/>
+      <c r="I382" s="168"/>
+      <c r="J382" s="168"/>
+      <c r="K382" s="168"/>
       <c r="L382" s="22"/>
       <c r="M382" s="34"/>
       <c r="N382" s="34"/>
@@ -8715,14 +8715,14 @@
       <c r="C383" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="D383" s="266"/>
-      <c r="E383" s="266"/>
-      <c r="F383" s="267"/>
-      <c r="G383" s="267"/>
-      <c r="H383" s="267"/>
-      <c r="I383" s="267"/>
-      <c r="J383" s="267"/>
-      <c r="K383" s="267"/>
+      <c r="D383" s="169"/>
+      <c r="E383" s="169"/>
+      <c r="F383" s="168"/>
+      <c r="G383" s="168"/>
+      <c r="H383" s="168"/>
+      <c r="I383" s="168"/>
+      <c r="J383" s="168"/>
+      <c r="K383" s="168"/>
       <c r="L383" s="22"/>
       <c r="M383" s="34"/>
       <c r="N383" s="34"/>
@@ -8847,10 +8847,10 @@
     </row>
     <row r="393" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B393" s="18"/>
-      <c r="D393" s="266" t="s">
+      <c r="D393" s="169" t="s">
         <v>265</v>
       </c>
-      <c r="E393" s="266"/>
+      <c r="E393" s="169"/>
       <c r="J393" s="25"/>
       <c r="K393" s="25"/>
       <c r="L393" s="25"/>
@@ -8858,43 +8858,43 @@
     </row>
     <row r="394" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B394" s="18"/>
-      <c r="C394" s="169" t="s">
+      <c r="C394" s="183" t="s">
         <v>182</v>
       </c>
-      <c r="D394" s="169" t="s">
+      <c r="D394" s="183" t="s">
         <v>264</v>
       </c>
-      <c r="E394" s="169" t="s">
+      <c r="E394" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="F394" s="169" t="s">
+      <c r="F394" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="G394" s="268" t="s">
+      <c r="G394" s="184" t="s">
         <v>183</v>
       </c>
-      <c r="H394" s="268" t="s">
+      <c r="H394" s="184" t="s">
         <v>176</v>
       </c>
-      <c r="I394" s="268" t="s">
+      <c r="I394" s="184" t="s">
         <v>184</v>
       </c>
-      <c r="J394" s="267" t="s">
+      <c r="J394" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="K394" s="267"/>
+      <c r="K394" s="168"/>
       <c r="L394" s="22"/>
       <c r="M394" s="25"/>
     </row>
     <row r="395" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B395" s="18"/>
-      <c r="C395" s="169"/>
-      <c r="D395" s="169"/>
-      <c r="E395" s="169"/>
-      <c r="F395" s="169"/>
-      <c r="G395" s="269"/>
-      <c r="H395" s="269"/>
-      <c r="I395" s="269"/>
+      <c r="C395" s="183"/>
+      <c r="D395" s="183"/>
+      <c r="E395" s="183"/>
+      <c r="F395" s="183"/>
+      <c r="G395" s="185"/>
+      <c r="H395" s="185"/>
+      <c r="I395" s="185"/>
       <c r="J395" s="75" t="s">
         <v>186</v>
       </c>
@@ -9199,21 +9199,21 @@
     </row>
     <row r="415" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="B415" s="18"/>
-      <c r="C415" s="192" t="s">
+      <c r="C415" s="179" t="s">
         <v>265</v>
       </c>
-      <c r="D415" s="194"/>
-      <c r="E415" s="192" t="s">
+      <c r="D415" s="181"/>
+      <c r="E415" s="179" t="s">
         <v>204</v>
       </c>
-      <c r="F415" s="193"/>
-      <c r="G415" s="193"/>
-      <c r="H415" s="193"/>
-      <c r="I415" s="193"/>
-      <c r="J415" s="193"/>
-      <c r="K415" s="194"/>
+      <c r="F415" s="180"/>
+      <c r="G415" s="180"/>
+      <c r="H415" s="180"/>
+      <c r="I415" s="180"/>
+      <c r="J415" s="180"/>
+      <c r="K415" s="181"/>
       <c r="L415" s="154"/>
-      <c r="M415" s="268" t="s">
+      <c r="M415" s="184" t="s">
         <v>205</v>
       </c>
     </row>
@@ -9247,7 +9247,7 @@
         <v>180</v>
       </c>
       <c r="L416" s="160"/>
-      <c r="M416" s="269"/>
+      <c r="M416" s="185"/>
     </row>
     <row r="417" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B417" s="20"/>
@@ -9493,23 +9493,23 @@
     </row>
     <row r="432" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B432" s="20"/>
-      <c r="C432" s="192" t="s">
+      <c r="C432" s="179" t="s">
         <v>265</v>
       </c>
-      <c r="D432" s="194"/>
-      <c r="E432" s="270" t="s">
+      <c r="D432" s="181"/>
+      <c r="E432" s="190" t="s">
         <v>214</v>
       </c>
-      <c r="F432" s="192" t="s">
+      <c r="F432" s="179" t="s">
         <v>204</v>
       </c>
-      <c r="G432" s="193"/>
-      <c r="H432" s="193"/>
-      <c r="I432" s="193"/>
-      <c r="J432" s="193"/>
-      <c r="K432" s="194"/>
+      <c r="G432" s="180"/>
+      <c r="H432" s="180"/>
+      <c r="I432" s="180"/>
+      <c r="J432" s="180"/>
+      <c r="K432" s="181"/>
       <c r="L432" s="154"/>
-      <c r="M432" s="268" t="s">
+      <c r="M432" s="184" t="s">
         <v>210</v>
       </c>
     </row>
@@ -9521,7 +9521,7 @@
       <c r="D433" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="E433" s="266"/>
+      <c r="E433" s="169"/>
       <c r="F433" s="75">
         <v>1</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>180</v>
       </c>
       <c r="L433" s="160"/>
-      <c r="M433" s="269"/>
+      <c r="M433" s="185"/>
     </row>
     <row r="434" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B434" s="20"/>
@@ -9729,26 +9729,26 @@
     </row>
     <row r="446" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B446" s="20"/>
-      <c r="C446" s="271" t="s">
+      <c r="C446" s="175" t="s">
         <v>59</v>
       </c>
-      <c r="D446" s="272"/>
-      <c r="E446" s="192" t="s">
+      <c r="D446" s="176"/>
+      <c r="E446" s="179" t="s">
         <v>204</v>
       </c>
-      <c r="F446" s="193"/>
-      <c r="G446" s="193"/>
-      <c r="H446" s="193"/>
-      <c r="I446" s="193"/>
-      <c r="J446" s="193"/>
-      <c r="K446" s="194"/>
+      <c r="F446" s="180"/>
+      <c r="G446" s="180"/>
+      <c r="H446" s="180"/>
+      <c r="I446" s="180"/>
+      <c r="J446" s="180"/>
+      <c r="K446" s="181"/>
       <c r="L446" s="22"/>
-      <c r="M446" s="275"/>
+      <c r="M446" s="182"/>
     </row>
     <row r="447" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B447" s="20"/>
-      <c r="C447" s="273"/>
-      <c r="D447" s="274"/>
+      <c r="C447" s="177"/>
+      <c r="D447" s="178"/>
       <c r="E447" s="75">
         <v>1</v>
       </c>
@@ -9771,14 +9771,14 @@
         <v>180</v>
       </c>
       <c r="L447" s="22"/>
-      <c r="M447" s="275"/>
+      <c r="M447" s="182"/>
     </row>
     <row r="448" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B448" s="20"/>
-      <c r="C448" s="208" t="s">
+      <c r="C448" s="170" t="s">
         <v>219</v>
       </c>
-      <c r="D448" s="209"/>
+      <c r="D448" s="171"/>
       <c r="E448" s="82"/>
       <c r="F448" s="82"/>
       <c r="G448" s="82"/>
@@ -9790,10 +9790,10 @@
     </row>
     <row r="449" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B449" s="20"/>
-      <c r="C449" s="208" t="s">
+      <c r="C449" s="170" t="s">
         <v>178</v>
       </c>
-      <c r="D449" s="209"/>
+      <c r="D449" s="171"/>
       <c r="E449" s="82"/>
       <c r="F449" s="82"/>
       <c r="G449" s="82"/>
@@ -9805,10 +9805,10 @@
     </row>
     <row r="450" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B450" s="20"/>
-      <c r="C450" s="208" t="s">
+      <c r="C450" s="170" t="s">
         <v>220</v>
       </c>
-      <c r="D450" s="209"/>
+      <c r="D450" s="171"/>
       <c r="E450" s="82"/>
       <c r="F450" s="82"/>
       <c r="G450" s="82"/>
@@ -9820,10 +9820,10 @@
     </row>
     <row r="451" spans="2:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B451" s="20"/>
-      <c r="C451" s="192" t="s">
+      <c r="C451" s="179" t="s">
         <v>210</v>
       </c>
-      <c r="D451" s="194"/>
+      <c r="D451" s="181"/>
       <c r="E451" s="46"/>
       <c r="F451" s="46"/>
       <c r="G451" s="46"/>
@@ -10159,17 +10159,17 @@
         <v>238</v>
       </c>
       <c r="C473" s="80"/>
-      <c r="E473" s="276" t="s">
+      <c r="E473" s="189" t="s">
         <v>328</v>
       </c>
-      <c r="F473" s="276"/>
-      <c r="G473" s="276"/>
-      <c r="H473" s="276"/>
-      <c r="I473" s="276"/>
-      <c r="J473" s="276"/>
-      <c r="K473" s="276"/>
-      <c r="L473" s="276"/>
-      <c r="M473" s="276"/>
+      <c r="F473" s="189"/>
+      <c r="G473" s="189"/>
+      <c r="H473" s="189"/>
+      <c r="I473" s="189"/>
+      <c r="J473" s="189"/>
+      <c r="K473" s="189"/>
+      <c r="L473" s="189"/>
+      <c r="M473" s="189"/>
       <c r="N473" s="134"/>
     </row>
     <row r="474" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10205,10 +10205,10 @@
     <row r="476" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B476" s="19"/>
       <c r="C476" s="19"/>
-      <c r="D476" s="266" t="s">
+      <c r="D476" s="169" t="s">
         <v>265</v>
       </c>
-      <c r="E476" s="266"/>
+      <c r="E476" s="169"/>
       <c r="F476" s="19"/>
       <c r="G476" s="19"/>
       <c r="H476" s="19"/>
@@ -10220,43 +10220,43 @@
     </row>
     <row r="477" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B477" s="79"/>
-      <c r="C477" s="169" t="s">
+      <c r="C477" s="183" t="s">
         <v>182</v>
       </c>
-      <c r="D477" s="169" t="s">
+      <c r="D477" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="E477" s="169" t="s">
+      <c r="E477" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="F477" s="169" t="s">
+      <c r="F477" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="G477" s="268" t="s">
+      <c r="G477" s="184" t="s">
         <v>183</v>
       </c>
-      <c r="H477" s="268" t="s">
+      <c r="H477" s="184" t="s">
         <v>176</v>
       </c>
-      <c r="I477" s="268" t="s">
+      <c r="I477" s="184" t="s">
         <v>184</v>
       </c>
-      <c r="J477" s="203" t="s">
+      <c r="J477" s="186" t="s">
         <v>240</v>
       </c>
-      <c r="K477" s="204"/>
-      <c r="L477" s="204"/>
-      <c r="M477" s="205"/>
+      <c r="K477" s="187"/>
+      <c r="L477" s="187"/>
+      <c r="M477" s="188"/>
     </row>
     <row r="478" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B478" s="79"/>
-      <c r="C478" s="169"/>
-      <c r="D478" s="169"/>
-      <c r="E478" s="169"/>
-      <c r="F478" s="169"/>
-      <c r="G478" s="269"/>
-      <c r="H478" s="269"/>
-      <c r="I478" s="269"/>
+      <c r="C478" s="183"/>
+      <c r="D478" s="183"/>
+      <c r="E478" s="183"/>
+      <c r="F478" s="183"/>
+      <c r="G478" s="185"/>
+      <c r="H478" s="185"/>
+      <c r="I478" s="185"/>
       <c r="J478" s="77" t="s">
         <v>241</v>
       </c>
@@ -10396,10 +10396,10 @@
       <c r="D485" s="80"/>
       <c r="E485" s="80"/>
       <c r="F485" s="40"/>
-      <c r="G485" s="279" t="s">
+      <c r="G485" s="161" t="s">
         <v>277</v>
       </c>
-      <c r="H485" s="279"/>
+      <c r="H485" s="161"/>
       <c r="I485" s="128">
         <v>10000</v>
       </c>
@@ -10418,10 +10418,10 @@
       <c r="D486" s="80"/>
       <c r="E486" s="80"/>
       <c r="F486" s="40"/>
-      <c r="G486" s="280" t="s">
+      <c r="G486" s="162" t="s">
         <v>278</v>
       </c>
-      <c r="H486" s="280"/>
+      <c r="H486" s="162"/>
       <c r="I486" s="128">
         <v>24961.5</v>
       </c>
@@ -10443,10 +10443,10 @@
       <c r="D487" s="80"/>
       <c r="E487" s="80"/>
       <c r="F487" s="40"/>
-      <c r="G487" s="280" t="s">
+      <c r="G487" s="162" t="s">
         <v>195</v>
       </c>
-      <c r="H487" s="280"/>
+      <c r="H487" s="162"/>
       <c r="I487" s="128">
         <v>17290.75</v>
       </c>
@@ -10465,10 +10465,10 @@
       <c r="D488" s="80"/>
       <c r="E488" s="80"/>
       <c r="F488" s="40"/>
-      <c r="G488" s="278" t="s">
+      <c r="G488" s="174" t="s">
         <v>196</v>
       </c>
-      <c r="H488" s="278"/>
+      <c r="H488" s="174"/>
       <c r="I488" s="129">
         <f>SUM(I479:I487)</f>
         <v>432791.55</v>
@@ -10613,27 +10613,27 @@
     </row>
     <row r="497" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B497" s="20"/>
-      <c r="C497" s="271" t="s">
+      <c r="C497" s="175" t="s">
         <v>59</v>
       </c>
-      <c r="D497" s="272"/>
-      <c r="E497" s="192" t="s">
+      <c r="D497" s="176"/>
+      <c r="E497" s="179" t="s">
         <v>204</v>
       </c>
-      <c r="F497" s="193"/>
-      <c r="G497" s="193"/>
-      <c r="H497" s="193"/>
-      <c r="I497" s="193"/>
-      <c r="J497" s="193"/>
-      <c r="K497" s="194"/>
+      <c r="F497" s="180"/>
+      <c r="G497" s="180"/>
+      <c r="H497" s="180"/>
+      <c r="I497" s="180"/>
+      <c r="J497" s="180"/>
+      <c r="K497" s="181"/>
       <c r="L497" s="22"/>
-      <c r="M497" s="275"/>
+      <c r="M497" s="182"/>
       <c r="N497" s="80"/>
     </row>
     <row r="498" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B498" s="20"/>
-      <c r="C498" s="273"/>
-      <c r="D498" s="274"/>
+      <c r="C498" s="177"/>
+      <c r="D498" s="178"/>
       <c r="E498" s="75">
         <v>1</v>
       </c>
@@ -10656,15 +10656,15 @@
         <v>10</v>
       </c>
       <c r="L498" s="22"/>
-      <c r="M498" s="275"/>
+      <c r="M498" s="182"/>
       <c r="N498" s="80"/>
     </row>
     <row r="499" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B499" s="20"/>
-      <c r="C499" s="208" t="s">
+      <c r="C499" s="170" t="s">
         <v>324</v>
       </c>
-      <c r="D499" s="209"/>
+      <c r="D499" s="171"/>
       <c r="E499" s="103"/>
       <c r="F499" s="103">
         <v>3500</v>
@@ -10686,10 +10686,10 @@
     </row>
     <row r="500" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B500" s="20"/>
-      <c r="C500" s="208" t="s">
+      <c r="C500" s="170" t="s">
         <v>178</v>
       </c>
-      <c r="D500" s="209"/>
+      <c r="D500" s="171"/>
       <c r="E500" s="82"/>
       <c r="F500" s="82"/>
       <c r="G500" s="82"/>
@@ -10703,10 +10703,10 @@
     </row>
     <row r="501" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B501" s="20"/>
-      <c r="C501" s="208" t="s">
+      <c r="C501" s="170" t="s">
         <v>220</v>
       </c>
-      <c r="D501" s="209"/>
+      <c r="D501" s="171"/>
       <c r="E501" s="82"/>
       <c r="F501" s="82"/>
       <c r="G501" s="82"/>
@@ -11190,12 +11190,12 @@
       <c r="M532" s="80"/>
     </row>
     <row r="533" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B533" s="222" t="s">
+      <c r="B533" s="172" t="s">
         <v>246</v>
       </c>
-      <c r="C533" s="222"/>
-      <c r="D533" s="222"/>
-      <c r="E533" s="222"/>
+      <c r="C533" s="172"/>
+      <c r="D533" s="172"/>
+      <c r="E533" s="172"/>
       <c r="J533" s="80"/>
       <c r="K533" s="80"/>
       <c r="L533" s="152"/>
@@ -11273,36 +11273,36 @@
       <c r="L538" s="151"/>
     </row>
     <row r="539" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B539" s="277" t="s">
+      <c r="B539" s="173" t="s">
         <v>248</v>
       </c>
-      <c r="C539" s="277"/>
-      <c r="D539" s="277"/>
-      <c r="E539" s="277"/>
-      <c r="F539" s="277"/>
-      <c r="G539" s="277"/>
-      <c r="H539" s="277"/>
-      <c r="I539" s="277"/>
-      <c r="J539" s="277"/>
-      <c r="K539" s="277"/>
-      <c r="L539" s="277"/>
-      <c r="M539" s="277"/>
+      <c r="C539" s="173"/>
+      <c r="D539" s="173"/>
+      <c r="E539" s="173"/>
+      <c r="F539" s="173"/>
+      <c r="G539" s="173"/>
+      <c r="H539" s="173"/>
+      <c r="I539" s="173"/>
+      <c r="J539" s="173"/>
+      <c r="K539" s="173"/>
+      <c r="L539" s="173"/>
+      <c r="M539" s="173"/>
     </row>
     <row r="540" spans="2:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B540" s="277" t="s">
+      <c r="B540" s="173" t="s">
         <v>271</v>
       </c>
-      <c r="C540" s="277"/>
-      <c r="D540" s="277"/>
-      <c r="E540" s="277"/>
-      <c r="F540" s="277"/>
-      <c r="G540" s="277"/>
-      <c r="H540" s="277"/>
-      <c r="I540" s="277"/>
-      <c r="J540" s="277"/>
-      <c r="K540" s="277"/>
-      <c r="L540" s="277"/>
-      <c r="M540" s="277"/>
+      <c r="C540" s="173"/>
+      <c r="D540" s="173"/>
+      <c r="E540" s="173"/>
+      <c r="F540" s="173"/>
+      <c r="G540" s="173"/>
+      <c r="H540" s="173"/>
+      <c r="I540" s="173"/>
+      <c r="J540" s="173"/>
+      <c r="K540" s="173"/>
+      <c r="L540" s="173"/>
+      <c r="M540" s="173"/>
     </row>
     <row r="541" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B541" s="80"/>
@@ -11333,20 +11333,20 @@
       <c r="L542" s="151"/>
     </row>
     <row r="543" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B543" s="277" t="s">
+      <c r="B543" s="173" t="s">
         <v>250</v>
       </c>
-      <c r="C543" s="277"/>
-      <c r="D543" s="277"/>
-      <c r="E543" s="277"/>
-      <c r="F543" s="277"/>
-      <c r="G543" s="277"/>
-      <c r="H543" s="277"/>
-      <c r="I543" s="277"/>
-      <c r="J543" s="277"/>
-      <c r="K543" s="277"/>
-      <c r="L543" s="277"/>
-      <c r="M543" s="277"/>
+      <c r="C543" s="173"/>
+      <c r="D543" s="173"/>
+      <c r="E543" s="173"/>
+      <c r="F543" s="173"/>
+      <c r="G543" s="173"/>
+      <c r="H543" s="173"/>
+      <c r="I543" s="173"/>
+      <c r="J543" s="173"/>
+      <c r="K543" s="173"/>
+      <c r="L543" s="173"/>
+      <c r="M543" s="173"/>
     </row>
     <row r="544" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B544" s="79"/>
@@ -11362,6 +11362,133 @@
     </row>
   </sheetData>
   <mergeCells count="151">
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="C285:F285"/>
+    <mergeCell ref="C286:F286"/>
+    <mergeCell ref="C270:D270"/>
+    <mergeCell ref="C271:D271"/>
+    <mergeCell ref="C272:D272"/>
+    <mergeCell ref="C246:M246"/>
+    <mergeCell ref="C247:M247"/>
+    <mergeCell ref="C269:D269"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="C236:M238"/>
+    <mergeCell ref="C261:M265"/>
+    <mergeCell ref="C277:M281"/>
+    <mergeCell ref="E269:M269"/>
+    <mergeCell ref="C273:D273"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="C88:K88"/>
+    <mergeCell ref="C220:D220"/>
+    <mergeCell ref="C228:M228"/>
+    <mergeCell ref="C152:F152"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="C182:G182"/>
+    <mergeCell ref="C186:G186"/>
+    <mergeCell ref="C370:M370"/>
+    <mergeCell ref="C350:G350"/>
+    <mergeCell ref="C352:G352"/>
+    <mergeCell ref="C354:G354"/>
+    <mergeCell ref="C154:G154"/>
+    <mergeCell ref="C369:D369"/>
+    <mergeCell ref="C346:F346"/>
+    <mergeCell ref="C348:F348"/>
+    <mergeCell ref="C287:F287"/>
+    <mergeCell ref="C288:F288"/>
+    <mergeCell ref="C289:F289"/>
+    <mergeCell ref="C291:F291"/>
+    <mergeCell ref="C293:F293"/>
+    <mergeCell ref="C328:M328"/>
+    <mergeCell ref="C342:M342"/>
+    <mergeCell ref="C359:M363"/>
+    <mergeCell ref="C300:M304"/>
+    <mergeCell ref="C307:M311"/>
+    <mergeCell ref="C322:M326"/>
+    <mergeCell ref="C336:M340"/>
+    <mergeCell ref="C368:D368"/>
+    <mergeCell ref="E368:M368"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C215:M217"/>
+    <mergeCell ref="C127:M127"/>
+    <mergeCell ref="C130:M130"/>
+    <mergeCell ref="C144:M144"/>
+    <mergeCell ref="C146:E146"/>
+    <mergeCell ref="C148:E148"/>
+    <mergeCell ref="C150:E150"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C122:M124"/>
+    <mergeCell ref="C194:M198"/>
+    <mergeCell ref="C201:M205"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="C163:M163"/>
+    <mergeCell ref="C180:F180"/>
+    <mergeCell ref="D379:E379"/>
+    <mergeCell ref="F379:H379"/>
+    <mergeCell ref="I379:K379"/>
+    <mergeCell ref="D376:E376"/>
+    <mergeCell ref="F376:H376"/>
+    <mergeCell ref="I376:K376"/>
+    <mergeCell ref="D377:E377"/>
+    <mergeCell ref="F377:H377"/>
+    <mergeCell ref="I377:K377"/>
+    <mergeCell ref="D378:E378"/>
+    <mergeCell ref="F378:H378"/>
+    <mergeCell ref="I378:K378"/>
+    <mergeCell ref="I394:I395"/>
+    <mergeCell ref="J394:K394"/>
+    <mergeCell ref="C415:D415"/>
+    <mergeCell ref="E415:K415"/>
+    <mergeCell ref="M415:M416"/>
+    <mergeCell ref="C432:D432"/>
+    <mergeCell ref="E432:E433"/>
+    <mergeCell ref="F432:K432"/>
+    <mergeCell ref="M432:M433"/>
+    <mergeCell ref="C394:C395"/>
+    <mergeCell ref="D394:D395"/>
+    <mergeCell ref="E394:E395"/>
+    <mergeCell ref="F394:F395"/>
+    <mergeCell ref="G394:G395"/>
+    <mergeCell ref="H394:H395"/>
+    <mergeCell ref="C451:D451"/>
+    <mergeCell ref="C477:C478"/>
+    <mergeCell ref="D477:D478"/>
+    <mergeCell ref="E477:E478"/>
+    <mergeCell ref="F477:F478"/>
+    <mergeCell ref="G477:G478"/>
+    <mergeCell ref="C446:D447"/>
+    <mergeCell ref="E446:K446"/>
+    <mergeCell ref="M446:M447"/>
+    <mergeCell ref="C448:D448"/>
+    <mergeCell ref="C449:D449"/>
+    <mergeCell ref="C450:D450"/>
+    <mergeCell ref="D476:E476"/>
+    <mergeCell ref="H477:H478"/>
+    <mergeCell ref="I477:I478"/>
+    <mergeCell ref="J477:M477"/>
+    <mergeCell ref="E473:M473"/>
+    <mergeCell ref="C501:D501"/>
+    <mergeCell ref="B533:E533"/>
+    <mergeCell ref="B539:M539"/>
+    <mergeCell ref="B540:M540"/>
+    <mergeCell ref="B543:M543"/>
+    <mergeCell ref="G488:H488"/>
+    <mergeCell ref="C497:D498"/>
+    <mergeCell ref="E497:K497"/>
+    <mergeCell ref="M497:M498"/>
+    <mergeCell ref="C499:D499"/>
+    <mergeCell ref="C500:D500"/>
     <mergeCell ref="G485:H485"/>
     <mergeCell ref="G486:H486"/>
     <mergeCell ref="G487:H487"/>
@@ -11386,133 +11513,6 @@
     <mergeCell ref="D381:E381"/>
     <mergeCell ref="F381:H381"/>
     <mergeCell ref="I381:K381"/>
-    <mergeCell ref="C501:D501"/>
-    <mergeCell ref="B533:E533"/>
-    <mergeCell ref="B539:M539"/>
-    <mergeCell ref="B540:M540"/>
-    <mergeCell ref="B543:M543"/>
-    <mergeCell ref="G488:H488"/>
-    <mergeCell ref="C497:D498"/>
-    <mergeCell ref="E497:K497"/>
-    <mergeCell ref="M497:M498"/>
-    <mergeCell ref="C499:D499"/>
-    <mergeCell ref="C500:D500"/>
-    <mergeCell ref="C451:D451"/>
-    <mergeCell ref="C477:C478"/>
-    <mergeCell ref="D477:D478"/>
-    <mergeCell ref="E477:E478"/>
-    <mergeCell ref="F477:F478"/>
-    <mergeCell ref="G477:G478"/>
-    <mergeCell ref="C446:D447"/>
-    <mergeCell ref="E446:K446"/>
-    <mergeCell ref="M446:M447"/>
-    <mergeCell ref="C448:D448"/>
-    <mergeCell ref="C449:D449"/>
-    <mergeCell ref="C450:D450"/>
-    <mergeCell ref="D476:E476"/>
-    <mergeCell ref="H477:H478"/>
-    <mergeCell ref="I477:I478"/>
-    <mergeCell ref="J477:M477"/>
-    <mergeCell ref="E473:M473"/>
-    <mergeCell ref="I394:I395"/>
-    <mergeCell ref="J394:K394"/>
-    <mergeCell ref="C415:D415"/>
-    <mergeCell ref="E415:K415"/>
-    <mergeCell ref="M415:M416"/>
-    <mergeCell ref="C432:D432"/>
-    <mergeCell ref="E432:E433"/>
-    <mergeCell ref="F432:K432"/>
-    <mergeCell ref="M432:M433"/>
-    <mergeCell ref="C394:C395"/>
-    <mergeCell ref="D394:D395"/>
-    <mergeCell ref="E394:E395"/>
-    <mergeCell ref="F394:F395"/>
-    <mergeCell ref="G394:G395"/>
-    <mergeCell ref="H394:H395"/>
-    <mergeCell ref="D379:E379"/>
-    <mergeCell ref="F379:H379"/>
-    <mergeCell ref="I379:K379"/>
-    <mergeCell ref="D376:E376"/>
-    <mergeCell ref="F376:H376"/>
-    <mergeCell ref="I376:K376"/>
-    <mergeCell ref="D377:E377"/>
-    <mergeCell ref="F377:H377"/>
-    <mergeCell ref="I377:K377"/>
-    <mergeCell ref="D378:E378"/>
-    <mergeCell ref="F378:H378"/>
-    <mergeCell ref="I378:K378"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C215:M217"/>
-    <mergeCell ref="C127:M127"/>
-    <mergeCell ref="C130:M130"/>
-    <mergeCell ref="C144:M144"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="C148:E148"/>
-    <mergeCell ref="C150:E150"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C122:M124"/>
-    <mergeCell ref="C194:M198"/>
-    <mergeCell ref="C201:M205"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="C163:M163"/>
-    <mergeCell ref="C180:F180"/>
-    <mergeCell ref="C182:G182"/>
-    <mergeCell ref="C186:G186"/>
-    <mergeCell ref="C370:M370"/>
-    <mergeCell ref="C350:G350"/>
-    <mergeCell ref="C352:G352"/>
-    <mergeCell ref="C354:G354"/>
-    <mergeCell ref="C154:G154"/>
-    <mergeCell ref="C369:D369"/>
-    <mergeCell ref="C346:F346"/>
-    <mergeCell ref="C348:F348"/>
-    <mergeCell ref="C287:F287"/>
-    <mergeCell ref="C288:F288"/>
-    <mergeCell ref="C289:F289"/>
-    <mergeCell ref="C291:F291"/>
-    <mergeCell ref="C293:F293"/>
-    <mergeCell ref="C328:M328"/>
-    <mergeCell ref="C342:M342"/>
-    <mergeCell ref="C359:M363"/>
-    <mergeCell ref="C300:M304"/>
-    <mergeCell ref="C307:M311"/>
-    <mergeCell ref="C322:M326"/>
-    <mergeCell ref="C336:M340"/>
-    <mergeCell ref="C368:D368"/>
-    <mergeCell ref="E368:M368"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="C285:F285"/>
-    <mergeCell ref="C286:F286"/>
-    <mergeCell ref="C270:D270"/>
-    <mergeCell ref="C271:D271"/>
-    <mergeCell ref="C272:D272"/>
-    <mergeCell ref="C246:M246"/>
-    <mergeCell ref="C247:M247"/>
-    <mergeCell ref="C269:D269"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="C236:M238"/>
-    <mergeCell ref="C261:M265"/>
-    <mergeCell ref="C277:M281"/>
-    <mergeCell ref="E269:M269"/>
-    <mergeCell ref="C273:D273"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="C88:K88"/>
-    <mergeCell ref="C220:D220"/>
-    <mergeCell ref="C228:M228"/>
-    <mergeCell ref="C152:F152"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G73:I73"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>